<commit_message>
Updated AttendanceTracker 01/27 12:29pm
</commit_message>
<xml_diff>
--- a/AttendanceTracker.xlsx
+++ b/AttendanceTracker.xlsx
@@ -4093,11 +4093,23 @@
       <c r="AF40" s="39" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="24" t="n"/>
+      <c r="A41" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-22</t>
+        </is>
+      </c>
       <c r="B41" s="212" t="n"/>
-      <c r="C41" s="212" t="n"/>
+      <c r="C41" s="212" t="inlineStr">
+        <is>
+          <t>0.95</t>
+        </is>
+      </c>
       <c r="D41" s="25" t="n"/>
-      <c r="E41" s="26" t="n"/>
+      <c r="E41" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F41" s="27" t="n"/>
       <c r="G41" s="210" t="n"/>
       <c r="H41" s="320" t="n"/>
@@ -4109,7 +4121,11 @@
       <c r="N41" s="210" t="n"/>
       <c r="O41" s="320" t="n"/>
       <c r="P41" s="319" t="n"/>
-      <c r="Q41" s="143" t="n"/>
+      <c r="Q41" s="143" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-09:57</t>
+        </is>
+      </c>
       <c r="R41" s="144" t="n"/>
       <c r="S41" s="144" t="n"/>
       <c r="T41" s="144" t="n"/>
@@ -4127,11 +4143,23 @@
       <c r="AF41" s="145" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="24" t="n"/>
+      <c r="A42" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
       <c r="B42" s="212" t="n"/>
-      <c r="C42" s="212" t="n"/>
+      <c r="C42" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D42" s="25" t="n"/>
-      <c r="E42" s="26" t="n"/>
+      <c r="E42" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F42" s="27" t="n"/>
       <c r="G42" s="210" t="n"/>
       <c r="H42" s="320" t="n"/>
@@ -4143,7 +4171,11 @@
       <c r="N42" s="210" t="n"/>
       <c r="O42" s="320" t="n"/>
       <c r="P42" s="319" t="n"/>
-      <c r="Q42" s="146" t="n"/>
+      <c r="Q42" s="146" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 09:00-19:15</t>
+        </is>
+      </c>
       <c r="R42" s="40" t="n"/>
       <c r="S42" s="40" t="n"/>
       <c r="T42" s="40" t="n"/>
@@ -5543,7 +5575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
@@ -6188,6 +6220,94 @@
         </is>
       </c>
       <c r="Q48" t="inlineStr">
+        <is>
+          <t>US Tardy 11:30-12:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>US Tardy 11:30-11:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-01-05</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>10.50</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 11:30-22:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-01-14</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>US Tardy 11:30-12:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1.08</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
         <is>
           <t>US Tardy 11:30-12:35</t>
         </is>
@@ -13280,10 +13400,22 @@
       <c r="AF128" s="319" t="n"/>
     </row>
     <row r="129">
-      <c r="A129" s="24" t="n"/>
+      <c r="A129" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-15</t>
+        </is>
+      </c>
       <c r="B129" s="212" t="inlineStr"/>
-      <c r="C129" s="212" t="n"/>
-      <c r="D129" s="212" t="n"/>
+      <c r="C129" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D129" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E129" s="320" t="n"/>
       <c r="F129" s="319" t="n"/>
       <c r="G129" s="210" t="n"/>
@@ -13296,7 +13428,11 @@
       <c r="N129" s="210" t="n"/>
       <c r="O129" s="320" t="n"/>
       <c r="P129" s="319" t="n"/>
-      <c r="Q129" s="253" t="n"/>
+      <c r="Q129" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R129" s="320" t="n"/>
       <c r="S129" s="320" t="n"/>
       <c r="T129" s="320" t="n"/>
@@ -13314,10 +13450,22 @@
       <c r="AF129" s="319" t="n"/>
     </row>
     <row r="130">
-      <c r="A130" s="24" t="n"/>
+      <c r="A130" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-16</t>
+        </is>
+      </c>
       <c r="B130" s="212" t="inlineStr"/>
-      <c r="C130" s="212" t="n"/>
-      <c r="D130" s="212" t="n"/>
+      <c r="C130" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D130" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E130" s="320" t="n"/>
       <c r="F130" s="319" t="n"/>
       <c r="G130" s="210" t="n"/>
@@ -13330,7 +13478,11 @@
       <c r="N130" s="210" t="n"/>
       <c r="O130" s="320" t="n"/>
       <c r="P130" s="319" t="n"/>
-      <c r="Q130" s="253" t="n"/>
+      <c r="Q130" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R130" s="320" t="n"/>
       <c r="S130" s="320" t="n"/>
       <c r="T130" s="320" t="n"/>
@@ -13348,10 +13500,22 @@
       <c r="AF130" s="319" t="n"/>
     </row>
     <row r="131">
-      <c r="A131" s="24" t="n"/>
+      <c r="A131" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B131" s="212" t="inlineStr"/>
-      <c r="C131" s="212" t="n"/>
-      <c r="D131" s="212" t="n"/>
+      <c r="C131" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D131" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E131" s="320" t="n"/>
       <c r="F131" s="319" t="n"/>
       <c r="G131" s="210" t="n"/>
@@ -13364,7 +13528,11 @@
       <c r="N131" s="210" t="n"/>
       <c r="O131" s="320" t="n"/>
       <c r="P131" s="319" t="n"/>
-      <c r="Q131" s="253" t="n"/>
+      <c r="Q131" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R131" s="320" t="n"/>
       <c r="S131" s="320" t="n"/>
       <c r="T131" s="320" t="n"/>
@@ -13382,10 +13550,22 @@
       <c r="AF131" s="319" t="n"/>
     </row>
     <row r="132">
-      <c r="A132" s="24" t="n"/>
+      <c r="A132" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-19</t>
+        </is>
+      </c>
       <c r="B132" s="212" t="inlineStr"/>
-      <c r="C132" s="212" t="n"/>
-      <c r="D132" s="212" t="n"/>
+      <c r="C132" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D132" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E132" s="320" t="n"/>
       <c r="F132" s="319" t="n"/>
       <c r="G132" s="210" t="n"/>
@@ -13398,7 +13578,11 @@
       <c r="N132" s="210" t="n"/>
       <c r="O132" s="320" t="n"/>
       <c r="P132" s="319" t="n"/>
-      <c r="Q132" s="253" t="n"/>
+      <c r="Q132" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R132" s="320" t="n"/>
       <c r="S132" s="320" t="n"/>
       <c r="T132" s="320" t="n"/>
@@ -13416,10 +13600,22 @@
       <c r="AF132" s="319" t="n"/>
     </row>
     <row r="133">
-      <c r="A133" s="24" t="n"/>
+      <c r="A133" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-20</t>
+        </is>
+      </c>
       <c r="B133" s="212" t="inlineStr"/>
-      <c r="C133" s="212" t="n"/>
-      <c r="D133" s="212" t="n"/>
+      <c r="C133" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D133" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E133" s="320" t="n"/>
       <c r="F133" s="319" t="n"/>
       <c r="G133" s="210" t="n"/>
@@ -13432,7 +13628,11 @@
       <c r="N133" s="210" t="n"/>
       <c r="O133" s="320" t="n"/>
       <c r="P133" s="319" t="n"/>
-      <c r="Q133" s="253" t="n"/>
+      <c r="Q133" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R133" s="320" t="n"/>
       <c r="S133" s="320" t="n"/>
       <c r="T133" s="320" t="n"/>
@@ -13450,10 +13650,22 @@
       <c r="AF133" s="319" t="n"/>
     </row>
     <row r="134">
-      <c r="A134" s="24" t="n"/>
+      <c r="A134" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-22</t>
+        </is>
+      </c>
       <c r="B134" s="212" t="inlineStr"/>
-      <c r="C134" s="212" t="n"/>
-      <c r="D134" s="212" t="n"/>
+      <c r="C134" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D134" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E134" s="320" t="n"/>
       <c r="F134" s="319" t="n"/>
       <c r="G134" s="210" t="n"/>
@@ -13466,7 +13678,11 @@
       <c r="N134" s="210" t="n"/>
       <c r="O134" s="320" t="n"/>
       <c r="P134" s="319" t="n"/>
-      <c r="Q134" s="253" t="n"/>
+      <c r="Q134" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R134" s="320" t="n"/>
       <c r="S134" s="320" t="n"/>
       <c r="T134" s="320" t="n"/>
@@ -13484,10 +13700,22 @@
       <c r="AF134" s="319" t="n"/>
     </row>
     <row r="135">
-      <c r="A135" s="24" t="n"/>
+      <c r="A135" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-23</t>
+        </is>
+      </c>
       <c r="B135" s="212" t="inlineStr"/>
-      <c r="C135" s="212" t="n"/>
-      <c r="D135" s="212" t="n"/>
+      <c r="C135" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D135" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E135" s="320" t="n"/>
       <c r="F135" s="319" t="n"/>
       <c r="G135" s="210" t="n"/>
@@ -13500,7 +13728,11 @@
       <c r="N135" s="210" t="n"/>
       <c r="O135" s="320" t="n"/>
       <c r="P135" s="319" t="n"/>
-      <c r="Q135" s="253" t="n"/>
+      <c r="Q135" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R135" s="320" t="n"/>
       <c r="S135" s="320" t="n"/>
       <c r="T135" s="320" t="n"/>
@@ -13518,10 +13750,22 @@
       <c r="AF135" s="319" t="n"/>
     </row>
     <row r="136">
-      <c r="A136" s="24" t="n"/>
+      <c r="A136" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-25</t>
+        </is>
+      </c>
       <c r="B136" s="212" t="inlineStr"/>
-      <c r="C136" s="212" t="n"/>
-      <c r="D136" s="212" t="n"/>
+      <c r="C136" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D136" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E136" s="320" t="n"/>
       <c r="F136" s="319" t="n"/>
       <c r="G136" s="210" t="n"/>
@@ -13534,7 +13778,11 @@
       <c r="N136" s="210" t="n"/>
       <c r="O136" s="320" t="n"/>
       <c r="P136" s="319" t="n"/>
-      <c r="Q136" s="253" t="n"/>
+      <c r="Q136" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R136" s="320" t="n"/>
       <c r="S136" s="320" t="n"/>
       <c r="T136" s="320" t="n"/>
@@ -13552,10 +13800,22 @@
       <c r="AF136" s="319" t="n"/>
     </row>
     <row r="137">
-      <c r="A137" s="24" t="n"/>
+      <c r="A137" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-26</t>
+        </is>
+      </c>
       <c r="B137" s="212" t="inlineStr"/>
-      <c r="C137" s="212" t="n"/>
-      <c r="D137" s="212" t="n"/>
+      <c r="C137" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D137" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E137" s="320" t="n"/>
       <c r="F137" s="319" t="n"/>
       <c r="G137" s="210" t="n"/>
@@ -13568,7 +13828,11 @@
       <c r="N137" s="210" t="n"/>
       <c r="O137" s="320" t="n"/>
       <c r="P137" s="319" t="n"/>
-      <c r="Q137" s="253" t="n"/>
+      <c r="Q137" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R137" s="320" t="n"/>
       <c r="S137" s="320" t="n"/>
       <c r="T137" s="320" t="n"/>
@@ -13586,10 +13850,22 @@
       <c r="AF137" s="319" t="n"/>
     </row>
     <row r="138">
-      <c r="A138" s="24" t="n"/>
+      <c r="A138" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-27</t>
+        </is>
+      </c>
       <c r="B138" s="212" t="inlineStr"/>
-      <c r="C138" s="212" t="n"/>
-      <c r="D138" s="212" t="n"/>
+      <c r="C138" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D138" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E138" s="320" t="n"/>
       <c r="F138" s="319" t="n"/>
       <c r="G138" s="210" t="n"/>
@@ -13602,7 +13878,11 @@
       <c r="N138" s="210" t="n"/>
       <c r="O138" s="320" t="n"/>
       <c r="P138" s="319" t="n"/>
-      <c r="Q138" s="253" t="n"/>
+      <c r="Q138" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R138" s="320" t="n"/>
       <c r="S138" s="320" t="n"/>
       <c r="T138" s="320" t="n"/>
@@ -13620,10 +13900,22 @@
       <c r="AF138" s="319" t="n"/>
     </row>
     <row r="139">
-      <c r="A139" s="24" t="n"/>
+      <c r="A139" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-29</t>
+        </is>
+      </c>
       <c r="B139" s="212" t="inlineStr"/>
-      <c r="C139" s="212" t="n"/>
-      <c r="D139" s="212" t="n"/>
+      <c r="C139" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D139" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E139" s="320" t="n"/>
       <c r="F139" s="319" t="n"/>
       <c r="G139" s="210" t="n"/>
@@ -13636,7 +13928,11 @@
       <c r="N139" s="210" t="n"/>
       <c r="O139" s="320" t="n"/>
       <c r="P139" s="319" t="n"/>
-      <c r="Q139" s="253" t="n"/>
+      <c r="Q139" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R139" s="320" t="n"/>
       <c r="S139" s="320" t="n"/>
       <c r="T139" s="320" t="n"/>
@@ -13654,10 +13950,22 @@
       <c r="AF139" s="319" t="n"/>
     </row>
     <row r="140">
-      <c r="A140" s="24" t="n"/>
+      <c r="A140" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-30</t>
+        </is>
+      </c>
       <c r="B140" s="212" t="inlineStr"/>
-      <c r="C140" s="212" t="n"/>
-      <c r="D140" s="212" t="n"/>
+      <c r="C140" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D140" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E140" s="320" t="n"/>
       <c r="F140" s="319" t="n"/>
       <c r="G140" s="210" t="n"/>
@@ -13670,7 +13978,11 @@
       <c r="N140" s="210" t="n"/>
       <c r="O140" s="320" t="n"/>
       <c r="P140" s="319" t="n"/>
-      <c r="Q140" s="253" t="n"/>
+      <c r="Q140" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R140" s="320" t="n"/>
       <c r="S140" s="320" t="n"/>
       <c r="T140" s="320" t="n"/>
@@ -13688,10 +14000,22 @@
       <c r="AF140" s="319" t="n"/>
     </row>
     <row r="141">
-      <c r="A141" s="24" t="n"/>
+      <c r="A141" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
       <c r="B141" s="212" t="inlineStr"/>
-      <c r="C141" s="212" t="n"/>
-      <c r="D141" s="212" t="n"/>
+      <c r="C141" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D141" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E141" s="320" t="n"/>
       <c r="F141" s="319" t="n"/>
       <c r="G141" s="210" t="n"/>
@@ -13704,7 +14028,11 @@
       <c r="N141" s="210" t="n"/>
       <c r="O141" s="320" t="n"/>
       <c r="P141" s="319" t="n"/>
-      <c r="Q141" s="253" t="n"/>
+      <c r="Q141" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R141" s="320" t="n"/>
       <c r="S141" s="320" t="n"/>
       <c r="T141" s="320" t="n"/>
@@ -13722,10 +14050,22 @@
       <c r="AF141" s="319" t="n"/>
     </row>
     <row r="142">
-      <c r="A142" s="24" t="n"/>
+      <c r="A142" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-02</t>
+        </is>
+      </c>
       <c r="B142" s="212" t="inlineStr"/>
-      <c r="C142" s="212" t="n"/>
-      <c r="D142" s="212" t="n"/>
+      <c r="C142" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D142" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E142" s="320" t="n"/>
       <c r="F142" s="319" t="n"/>
       <c r="G142" s="210" t="n"/>
@@ -13738,7 +14078,11 @@
       <c r="N142" s="210" t="n"/>
       <c r="O142" s="320" t="n"/>
       <c r="P142" s="319" t="n"/>
-      <c r="Q142" s="253" t="n"/>
+      <c r="Q142" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R142" s="320" t="n"/>
       <c r="S142" s="320" t="n"/>
       <c r="T142" s="320" t="n"/>
@@ -13756,10 +14100,22 @@
       <c r="AF142" s="319" t="n"/>
     </row>
     <row r="143">
-      <c r="A143" s="24" t="n"/>
+      <c r="A143" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-03</t>
+        </is>
+      </c>
       <c r="B143" s="212" t="inlineStr"/>
-      <c r="C143" s="212" t="n"/>
-      <c r="D143" s="212" t="n"/>
+      <c r="C143" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D143" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E143" s="320" t="n"/>
       <c r="F143" s="319" t="n"/>
       <c r="G143" s="210" t="n"/>
@@ -13772,7 +14128,11 @@
       <c r="N143" s="210" t="n"/>
       <c r="O143" s="320" t="n"/>
       <c r="P143" s="319" t="n"/>
-      <c r="Q143" s="253" t="n"/>
+      <c r="Q143" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R143" s="320" t="n"/>
       <c r="S143" s="320" t="n"/>
       <c r="T143" s="320" t="n"/>
@@ -13790,10 +14150,22 @@
       <c r="AF143" s="319" t="n"/>
     </row>
     <row r="144">
-      <c r="A144" s="24" t="n"/>
+      <c r="A144" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-05</t>
+        </is>
+      </c>
       <c r="B144" s="212" t="inlineStr"/>
-      <c r="C144" s="212" t="n"/>
-      <c r="D144" s="212" t="n"/>
+      <c r="C144" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D144" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E144" s="320" t="n"/>
       <c r="F144" s="319" t="n"/>
       <c r="G144" s="210" t="n"/>
@@ -13806,7 +14178,11 @@
       <c r="N144" s="210" t="n"/>
       <c r="O144" s="320" t="n"/>
       <c r="P144" s="319" t="n"/>
-      <c r="Q144" s="253" t="n"/>
+      <c r="Q144" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R144" s="320" t="n"/>
       <c r="S144" s="320" t="n"/>
       <c r="T144" s="320" t="n"/>
@@ -13824,10 +14200,22 @@
       <c r="AF144" s="319" t="n"/>
     </row>
     <row r="145">
-      <c r="A145" s="24" t="n"/>
+      <c r="A145" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-06</t>
+        </is>
+      </c>
       <c r="B145" s="212" t="inlineStr"/>
-      <c r="C145" s="212" t="n"/>
-      <c r="D145" s="212" t="n"/>
+      <c r="C145" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D145" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E145" s="320" t="n"/>
       <c r="F145" s="319" t="n"/>
       <c r="G145" s="210" t="n"/>
@@ -13840,7 +14228,11 @@
       <c r="N145" s="210" t="n"/>
       <c r="O145" s="320" t="n"/>
       <c r="P145" s="319" t="n"/>
-      <c r="Q145" s="253" t="n"/>
+      <c r="Q145" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R145" s="320" t="n"/>
       <c r="S145" s="320" t="n"/>
       <c r="T145" s="320" t="n"/>
@@ -13858,10 +14250,22 @@
       <c r="AF145" s="319" t="n"/>
     </row>
     <row r="146">
-      <c r="A146" s="24" t="n"/>
+      <c r="A146" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
       <c r="B146" s="212" t="inlineStr"/>
-      <c r="C146" s="212" t="n"/>
-      <c r="D146" s="212" t="n"/>
+      <c r="C146" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D146" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E146" s="320" t="n"/>
       <c r="F146" s="319" t="n"/>
       <c r="G146" s="210" t="n"/>
@@ -13874,7 +14278,11 @@
       <c r="N146" s="210" t="n"/>
       <c r="O146" s="320" t="n"/>
       <c r="P146" s="319" t="n"/>
-      <c r="Q146" s="253" t="n"/>
+      <c r="Q146" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R146" s="320" t="n"/>
       <c r="S146" s="320" t="n"/>
       <c r="T146" s="320" t="n"/>
@@ -13892,10 +14300,22 @@
       <c r="AF146" s="319" t="n"/>
     </row>
     <row r="147">
-      <c r="A147" s="24" t="n"/>
+      <c r="A147" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-09</t>
+        </is>
+      </c>
       <c r="B147" s="212" t="inlineStr"/>
-      <c r="C147" s="212" t="n"/>
-      <c r="D147" s="212" t="n"/>
+      <c r="C147" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D147" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E147" s="320" t="n"/>
       <c r="F147" s="319" t="n"/>
       <c r="G147" s="210" t="n"/>
@@ -13908,7 +14328,11 @@
       <c r="N147" s="210" t="n"/>
       <c r="O147" s="320" t="n"/>
       <c r="P147" s="319" t="n"/>
-      <c r="Q147" s="253" t="n"/>
+      <c r="Q147" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R147" s="320" t="n"/>
       <c r="S147" s="320" t="n"/>
       <c r="T147" s="320" t="n"/>
@@ -13926,10 +14350,22 @@
       <c r="AF147" s="319" t="n"/>
     </row>
     <row r="148">
-      <c r="A148" s="24" t="n"/>
+      <c r="A148" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-10</t>
+        </is>
+      </c>
       <c r="B148" s="212" t="inlineStr"/>
-      <c r="C148" s="212" t="n"/>
-      <c r="D148" s="212" t="n"/>
+      <c r="C148" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D148" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E148" s="320" t="n"/>
       <c r="F148" s="319" t="n"/>
       <c r="G148" s="210" t="n"/>
@@ -13942,7 +14378,11 @@
       <c r="N148" s="210" t="n"/>
       <c r="O148" s="320" t="n"/>
       <c r="P148" s="319" t="n"/>
-      <c r="Q148" s="253" t="n"/>
+      <c r="Q148" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R148" s="320" t="n"/>
       <c r="S148" s="320" t="n"/>
       <c r="T148" s="320" t="n"/>
@@ -13960,10 +14400,22 @@
       <c r="AF148" s="319" t="n"/>
     </row>
     <row r="149">
-      <c r="A149" s="24" t="n"/>
+      <c r="A149" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-12</t>
+        </is>
+      </c>
       <c r="B149" s="212" t="inlineStr"/>
-      <c r="C149" s="212" t="n"/>
-      <c r="D149" s="212" t="n"/>
+      <c r="C149" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D149" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E149" s="320" t="n"/>
       <c r="F149" s="319" t="n"/>
       <c r="G149" s="210" t="n"/>
@@ -13976,7 +14428,11 @@
       <c r="N149" s="210" t="n"/>
       <c r="O149" s="320" t="n"/>
       <c r="P149" s="319" t="n"/>
-      <c r="Q149" s="253" t="n"/>
+      <c r="Q149" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R149" s="320" t="n"/>
       <c r="S149" s="320" t="n"/>
       <c r="T149" s="320" t="n"/>
@@ -13994,10 +14450,22 @@
       <c r="AF149" s="319" t="n"/>
     </row>
     <row r="150">
-      <c r="A150" s="24" t="n"/>
+      <c r="A150" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-13</t>
+        </is>
+      </c>
       <c r="B150" s="212" t="inlineStr"/>
-      <c r="C150" s="212" t="n"/>
-      <c r="D150" s="212" t="n"/>
+      <c r="C150" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D150" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E150" s="320" t="n"/>
       <c r="F150" s="319" t="n"/>
       <c r="G150" s="210" t="n"/>
@@ -14010,7 +14478,11 @@
       <c r="N150" s="210" t="n"/>
       <c r="O150" s="320" t="n"/>
       <c r="P150" s="319" t="n"/>
-      <c r="Q150" s="253" t="n"/>
+      <c r="Q150" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R150" s="320" t="n"/>
       <c r="S150" s="320" t="n"/>
       <c r="T150" s="320" t="n"/>
@@ -14028,10 +14500,22 @@
       <c r="AF150" s="319" t="n"/>
     </row>
     <row r="151">
-      <c r="A151" s="24" t="n"/>
+      <c r="A151" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
       <c r="B151" s="212" t="inlineStr"/>
-      <c r="C151" s="212" t="n"/>
-      <c r="D151" s="212" t="n"/>
+      <c r="C151" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D151" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E151" s="320" t="n"/>
       <c r="F151" s="319" t="n"/>
       <c r="G151" s="210" t="n"/>
@@ -14044,7 +14528,11 @@
       <c r="N151" s="210" t="n"/>
       <c r="O151" s="320" t="n"/>
       <c r="P151" s="319" t="n"/>
-      <c r="Q151" s="253" t="n"/>
+      <c r="Q151" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R151" s="320" t="n"/>
       <c r="S151" s="320" t="n"/>
       <c r="T151" s="320" t="n"/>
@@ -14062,10 +14550,22 @@
       <c r="AF151" s="319" t="n"/>
     </row>
     <row r="152">
-      <c r="A152" s="24" t="n"/>
+      <c r="A152" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-16</t>
+        </is>
+      </c>
       <c r="B152" s="212" t="inlineStr"/>
-      <c r="C152" s="212" t="n"/>
-      <c r="D152" s="212" t="n"/>
+      <c r="C152" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D152" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E152" s="320" t="n"/>
       <c r="F152" s="319" t="n"/>
       <c r="G152" s="210" t="n"/>
@@ -14078,7 +14578,11 @@
       <c r="N152" s="210" t="n"/>
       <c r="O152" s="320" t="n"/>
       <c r="P152" s="319" t="n"/>
-      <c r="Q152" s="253" t="n"/>
+      <c r="Q152" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R152" s="320" t="n"/>
       <c r="S152" s="320" t="n"/>
       <c r="T152" s="320" t="n"/>
@@ -14096,10 +14600,22 @@
       <c r="AF152" s="319" t="n"/>
     </row>
     <row r="153">
-      <c r="A153" s="24" t="n"/>
+      <c r="A153" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
       <c r="B153" s="212" t="inlineStr"/>
-      <c r="C153" s="212" t="n"/>
-      <c r="D153" s="212" t="n"/>
+      <c r="C153" s="212" t="inlineStr">
+        <is>
+          <t>6.50</t>
+        </is>
+      </c>
+      <c r="D153" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E153" s="320" t="n"/>
       <c r="F153" s="319" t="n"/>
       <c r="G153" s="210" t="n"/>
@@ -14112,7 +14628,11 @@
       <c r="N153" s="210" t="n"/>
       <c r="O153" s="320" t="n"/>
       <c r="P153" s="319" t="n"/>
-      <c r="Q153" s="253" t="n"/>
+      <c r="Q153" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-20:00</t>
+        </is>
+      </c>
       <c r="R153" s="320" t="n"/>
       <c r="S153" s="320" t="n"/>
       <c r="T153" s="320" t="n"/>
@@ -16958,11 +17478,23 @@
       <c r="AF45" s="33" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="24" t="n"/>
+      <c r="A46" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-16</t>
+        </is>
+      </c>
       <c r="B46" s="212" t="n"/>
-      <c r="C46" s="212" t="n"/>
+      <c r="C46" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D46" s="25" t="n"/>
-      <c r="E46" s="26" t="n"/>
+      <c r="E46" s="26" t="inlineStr">
+        <is>
+          <t>US Bereavement</t>
+        </is>
+      </c>
       <c r="F46" s="27" t="n"/>
       <c r="G46" s="210" t="n"/>
       <c r="H46" s="320" t="n"/>
@@ -16974,7 +17506,11 @@
       <c r="N46" s="210" t="n"/>
       <c r="O46" s="320" t="n"/>
       <c r="P46" s="319" t="n"/>
-      <c r="Q46" s="31" t="n"/>
+      <c r="Q46" s="31" t="inlineStr">
+        <is>
+          <t>US Bereavement 11:45-22:00</t>
+        </is>
+      </c>
       <c r="R46" s="32" t="n"/>
       <c r="S46" s="32" t="n"/>
       <c r="T46" s="32" t="n"/>
@@ -16992,11 +17528,23 @@
       <c r="AF46" s="33" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="24" t="n"/>
+      <c r="A47" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B47" s="212" t="n"/>
-      <c r="C47" s="212" t="n"/>
+      <c r="C47" s="212" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
       <c r="D47" s="25" t="n"/>
-      <c r="E47" s="26" t="n"/>
+      <c r="E47" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F47" s="27" t="n"/>
       <c r="G47" s="210" t="n"/>
       <c r="H47" s="320" t="n"/>
@@ -17008,7 +17556,11 @@
       <c r="N47" s="210" t="n"/>
       <c r="O47" s="320" t="n"/>
       <c r="P47" s="319" t="n"/>
-      <c r="Q47" s="31" t="n"/>
+      <c r="Q47" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 14:45-15:15</t>
+        </is>
+      </c>
       <c r="R47" s="32" t="n"/>
       <c r="S47" s="32" t="n"/>
       <c r="T47" s="32" t="n"/>
@@ -17026,11 +17578,23 @@
       <c r="AF47" s="33" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="24" t="n"/>
+      <c r="A48" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-23</t>
+        </is>
+      </c>
       <c r="B48" s="212" t="n"/>
-      <c r="C48" s="212" t="n"/>
+      <c r="C48" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D48" s="25" t="n"/>
-      <c r="E48" s="26" t="n"/>
+      <c r="E48" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F48" s="27" t="n"/>
       <c r="G48" s="210" t="n"/>
       <c r="H48" s="320" t="n"/>
@@ -17042,7 +17606,11 @@
       <c r="N48" s="210" t="n"/>
       <c r="O48" s="320" t="n"/>
       <c r="P48" s="319" t="n"/>
-      <c r="Q48" s="31" t="n"/>
+      <c r="Q48" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 11:45-22:00</t>
+        </is>
+      </c>
       <c r="R48" s="32" t="n"/>
       <c r="S48" s="32" t="n"/>
       <c r="T48" s="32" t="n"/>
@@ -17060,11 +17628,23 @@
       <c r="AF48" s="33" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="24" t="n"/>
+      <c r="A49" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-30</t>
+        </is>
+      </c>
       <c r="B49" s="212" t="n"/>
-      <c r="C49" s="212" t="n"/>
+      <c r="C49" s="212" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
       <c r="D49" s="25" t="n"/>
-      <c r="E49" s="26" t="n"/>
+      <c r="E49" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F49" s="27" t="n"/>
       <c r="G49" s="210" t="n"/>
       <c r="H49" s="320" t="n"/>
@@ -17076,7 +17656,11 @@
       <c r="N49" s="210" t="n"/>
       <c r="O49" s="320" t="n"/>
       <c r="P49" s="319" t="n"/>
-      <c r="Q49" s="31" t="n"/>
+      <c r="Q49" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 11:45-11:55</t>
+        </is>
+      </c>
       <c r="R49" s="32" t="n"/>
       <c r="S49" s="32" t="n"/>
       <c r="T49" s="32" t="n"/>
@@ -17094,11 +17678,23 @@
       <c r="AF49" s="33" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="24" t="n"/>
+      <c r="A50" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-10</t>
+        </is>
+      </c>
       <c r="B50" s="212" t="n"/>
-      <c r="C50" s="212" t="n"/>
+      <c r="C50" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D50" s="25" t="n"/>
-      <c r="E50" s="26" t="n"/>
+      <c r="E50" s="26" t="inlineStr">
+        <is>
+          <t>US NCL</t>
+        </is>
+      </c>
       <c r="F50" s="27" t="n"/>
       <c r="G50" s="210" t="n"/>
       <c r="H50" s="320" t="n"/>
@@ -17110,7 +17706,11 @@
       <c r="N50" s="210" t="n"/>
       <c r="O50" s="320" t="n"/>
       <c r="P50" s="319" t="n"/>
-      <c r="Q50" s="31" t="n"/>
+      <c r="Q50" s="31" t="inlineStr">
+        <is>
+          <t>US NCL 11:45-22:00</t>
+        </is>
+      </c>
       <c r="R50" s="32" t="n"/>
       <c r="S50" s="32" t="n"/>
       <c r="T50" s="32" t="n"/>
@@ -17128,11 +17728,23 @@
       <c r="AF50" s="33" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="24" t="n"/>
+      <c r="A51" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-13</t>
+        </is>
+      </c>
       <c r="B51" s="212" t="n"/>
-      <c r="C51" s="212" t="n"/>
+      <c r="C51" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D51" s="25" t="n"/>
-      <c r="E51" s="26" t="n"/>
+      <c r="E51" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F51" s="27" t="n"/>
       <c r="G51" s="210" t="n"/>
       <c r="H51" s="320" t="n"/>
@@ -17144,7 +17756,11 @@
       <c r="N51" s="210" t="n"/>
       <c r="O51" s="320" t="n"/>
       <c r="P51" s="319" t="n"/>
-      <c r="Q51" s="31" t="n"/>
+      <c r="Q51" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 11:45-22:00</t>
+        </is>
+      </c>
       <c r="R51" s="32" t="n"/>
       <c r="S51" s="32" t="n"/>
       <c r="T51" s="32" t="n"/>
@@ -21365,11 +21981,23 @@
       <c r="AF51" s="232" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="24" t="n"/>
+      <c r="A52" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-16</t>
+        </is>
+      </c>
       <c r="B52" s="212" t="n"/>
-      <c r="C52" s="212" t="n"/>
+      <c r="C52" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
       <c r="D52" s="212" t="n"/>
-      <c r="E52" s="212" t="n"/>
+      <c r="E52" s="212" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F52" s="212" t="n"/>
       <c r="G52" s="210" t="n"/>
       <c r="H52" s="320" t="n"/>
@@ -21381,7 +22009,11 @@
       <c r="N52" s="210" t="n"/>
       <c r="O52" s="320" t="n"/>
       <c r="P52" s="319" t="n"/>
-      <c r="Q52" s="232" t="n"/>
+      <c r="Q52" s="232" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R52" s="232" t="n"/>
       <c r="S52" s="232" t="n"/>
       <c r="T52" s="232" t="n"/>
@@ -21399,11 +22031,23 @@
       <c r="AF52" s="232" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="24" t="n"/>
+      <c r="A53" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-20</t>
+        </is>
+      </c>
       <c r="B53" s="212" t="n"/>
-      <c r="C53" s="212" t="n"/>
+      <c r="C53" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
       <c r="D53" s="212" t="n"/>
-      <c r="E53" s="212" t="n"/>
+      <c r="E53" s="212" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F53" s="212" t="n"/>
       <c r="G53" s="210" t="n"/>
       <c r="H53" s="320" t="n"/>
@@ -21415,7 +22059,11 @@
       <c r="N53" s="210" t="n"/>
       <c r="O53" s="320" t="n"/>
       <c r="P53" s="319" t="n"/>
-      <c r="Q53" s="232" t="n"/>
+      <c r="Q53" s="232" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R53" s="232" t="n"/>
       <c r="S53" s="232" t="n"/>
       <c r="T53" s="232" t="n"/>
@@ -21433,11 +22081,23 @@
       <c r="AF53" s="232" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="24" t="n"/>
+      <c r="A54" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
       <c r="B54" s="212" t="n"/>
-      <c r="C54" s="212" t="n"/>
+      <c r="C54" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
       <c r="D54" s="212" t="n"/>
-      <c r="E54" s="212" t="n"/>
+      <c r="E54" s="212" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F54" s="212" t="n"/>
       <c r="G54" s="210" t="n"/>
       <c r="H54" s="320" t="n"/>
@@ -21449,7 +22109,11 @@
       <c r="N54" s="210" t="n"/>
       <c r="O54" s="320" t="n"/>
       <c r="P54" s="319" t="n"/>
-      <c r="Q54" s="232" t="n"/>
+      <c r="Q54" s="232" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R54" s="232" t="n"/>
       <c r="S54" s="232" t="n"/>
       <c r="T54" s="232" t="n"/>
@@ -26966,11 +27630,23 @@
       <c r="AF38" s="33" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="24" t="n"/>
+      <c r="A39" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-16</t>
+        </is>
+      </c>
       <c r="B39" s="212" t="n"/>
-      <c r="C39" s="212" t="n"/>
+      <c r="C39" s="212" t="inlineStr">
+        <is>
+          <t>6.50</t>
+        </is>
+      </c>
       <c r="D39" s="25" t="n"/>
-      <c r="E39" s="26" t="n"/>
+      <c r="E39" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F39" s="27" t="n"/>
       <c r="G39" s="210" t="n"/>
       <c r="H39" s="320" t="n"/>
@@ -26982,7 +27658,11 @@
       <c r="N39" s="210" t="n"/>
       <c r="O39" s="320" t="n"/>
       <c r="P39" s="319" t="n"/>
-      <c r="Q39" s="31" t="n"/>
+      <c r="Q39" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 12:00-18:30</t>
+        </is>
+      </c>
       <c r="R39" s="32" t="n"/>
       <c r="S39" s="32" t="n"/>
       <c r="T39" s="32" t="n"/>
@@ -27000,11 +27680,23 @@
       <c r="AF39" s="33" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="24" t="n"/>
+      <c r="A40" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-30</t>
+        </is>
+      </c>
       <c r="B40" s="212" t="n"/>
-      <c r="C40" s="212" t="n"/>
+      <c r="C40" s="212" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
       <c r="D40" s="25" t="n"/>
-      <c r="E40" s="26" t="n"/>
+      <c r="E40" s="26" t="inlineStr">
+        <is>
+          <t>US NCL</t>
+        </is>
+      </c>
       <c r="F40" s="27" t="n"/>
       <c r="G40" s="210" t="n"/>
       <c r="H40" s="320" t="n"/>
@@ -27016,7 +27708,11 @@
       <c r="N40" s="210" t="n"/>
       <c r="O40" s="320" t="n"/>
       <c r="P40" s="319" t="n"/>
-      <c r="Q40" s="31" t="n"/>
+      <c r="Q40" s="31" t="inlineStr">
+        <is>
+          <t>US NCL 17:30-18:30</t>
+        </is>
+      </c>
       <c r="R40" s="32" t="n"/>
       <c r="S40" s="32" t="n"/>
       <c r="T40" s="32" t="n"/>
@@ -27034,11 +27730,23 @@
       <c r="AF40" s="33" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="54" t="n"/>
+      <c r="A41" s="54" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
       <c r="B41" s="211" t="n"/>
-      <c r="C41" s="211" t="n"/>
+      <c r="C41" s="211" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
       <c r="D41" s="78" t="n"/>
-      <c r="E41" s="77" t="n"/>
+      <c r="E41" s="77" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F41" s="76" t="n"/>
       <c r="G41" s="223" t="n"/>
       <c r="H41" s="320" t="n"/>
@@ -27050,7 +27758,11 @@
       <c r="N41" s="223" t="n"/>
       <c r="O41" s="320" t="n"/>
       <c r="P41" s="319" t="n"/>
-      <c r="Q41" s="280" t="n"/>
+      <c r="Q41" s="280" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-10:12</t>
+        </is>
+      </c>
       <c r="R41" s="74" t="n"/>
       <c r="S41" s="74" t="n"/>
       <c r="T41" s="74" t="n"/>
@@ -32169,11 +32881,23 @@
       <c r="AF56" s="33" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="24" t="n"/>
+      <c r="A57" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-17</t>
+        </is>
+      </c>
       <c r="B57" s="212" t="n"/>
-      <c r="C57" s="212" t="n"/>
+      <c r="C57" s="212" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
       <c r="D57" s="25" t="n"/>
-      <c r="E57" s="26" t="n"/>
+      <c r="E57" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F57" s="27" t="n"/>
       <c r="G57" s="210" t="n"/>
       <c r="H57" s="320" t="n"/>
@@ -32185,7 +32909,11 @@
       <c r="N57" s="210" t="n"/>
       <c r="O57" s="320" t="n"/>
       <c r="P57" s="319" t="n"/>
-      <c r="Q57" s="31" t="n"/>
+      <c r="Q57" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 10:30-11:34</t>
+        </is>
+      </c>
       <c r="R57" s="32" t="n"/>
       <c r="S57" s="32" t="n"/>
       <c r="T57" s="32" t="n"/>
@@ -32203,11 +32931,23 @@
       <c r="AF57" s="33" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="24" t="n"/>
+      <c r="A58" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-19</t>
+        </is>
+      </c>
       <c r="B58" s="212" t="n"/>
-      <c r="C58" s="212" t="n"/>
+      <c r="C58" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D58" s="25" t="n"/>
-      <c r="E58" s="26" t="n"/>
+      <c r="E58" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F58" s="27" t="n"/>
       <c r="G58" s="210" t="n"/>
       <c r="H58" s="320" t="n"/>
@@ -32219,7 +32959,11 @@
       <c r="N58" s="210" t="n"/>
       <c r="O58" s="320" t="n"/>
       <c r="P58" s="319" t="n"/>
-      <c r="Q58" s="31" t="n"/>
+      <c r="Q58" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R58" s="32" t="n"/>
       <c r="S58" s="32" t="n"/>
       <c r="T58" s="32" t="n"/>
@@ -32237,11 +32981,23 @@
       <c r="AF58" s="33" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="24" t="n"/>
+      <c r="A59" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-26</t>
+        </is>
+      </c>
       <c r="B59" s="212" t="n"/>
-      <c r="C59" s="212" t="n"/>
+      <c r="C59" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D59" s="25" t="n"/>
-      <c r="E59" s="26" t="n"/>
+      <c r="E59" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F59" s="27" t="n"/>
       <c r="G59" s="210" t="n"/>
       <c r="H59" s="320" t="n"/>
@@ -32253,7 +33009,11 @@
       <c r="N59" s="210" t="n"/>
       <c r="O59" s="320" t="n"/>
       <c r="P59" s="319" t="n"/>
-      <c r="Q59" s="31" t="n"/>
+      <c r="Q59" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R59" s="32" t="n"/>
       <c r="S59" s="32" t="n"/>
       <c r="T59" s="32" t="n"/>
@@ -32271,11 +33031,23 @@
       <c r="AF59" s="33" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="24" t="n"/>
+      <c r="A60" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-29</t>
+        </is>
+      </c>
       <c r="B60" s="212" t="n"/>
-      <c r="C60" s="212" t="n"/>
+      <c r="C60" s="212" t="inlineStr">
+        <is>
+          <t>3.67</t>
+        </is>
+      </c>
       <c r="D60" s="25" t="n"/>
-      <c r="E60" s="26" t="n"/>
+      <c r="E60" s="26" t="inlineStr">
+        <is>
+          <t>US Partial</t>
+        </is>
+      </c>
       <c r="F60" s="27" t="n"/>
       <c r="G60" s="210" t="n"/>
       <c r="H60" s="320" t="n"/>
@@ -32287,7 +33059,11 @@
       <c r="N60" s="210" t="n"/>
       <c r="O60" s="320" t="n"/>
       <c r="P60" s="319" t="n"/>
-      <c r="Q60" s="31" t="n"/>
+      <c r="Q60" s="31" t="inlineStr">
+        <is>
+          <t>US Partial 17:05-20:45</t>
+        </is>
+      </c>
       <c r="R60" s="32" t="n"/>
       <c r="S60" s="32" t="n"/>
       <c r="T60" s="32" t="n"/>
@@ -32305,11 +33081,23 @@
       <c r="AF60" s="33" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" s="24" t="n"/>
+      <c r="A61" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
       <c r="B61" s="212" t="n"/>
-      <c r="C61" s="212" t="n"/>
+      <c r="C61" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D61" s="25" t="n"/>
-      <c r="E61" s="26" t="n"/>
+      <c r="E61" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F61" s="27" t="n"/>
       <c r="G61" s="210" t="n"/>
       <c r="H61" s="320" t="n"/>
@@ -32321,7 +33109,11 @@
       <c r="N61" s="210" t="n"/>
       <c r="O61" s="320" t="n"/>
       <c r="P61" s="319" t="n"/>
-      <c r="Q61" s="31" t="n"/>
+      <c r="Q61" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R61" s="32" t="n"/>
       <c r="S61" s="32" t="n"/>
       <c r="T61" s="32" t="n"/>
@@ -32339,11 +33131,23 @@
       <c r="AF61" s="33" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" s="24" t="n"/>
+      <c r="A62" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-02</t>
+        </is>
+      </c>
       <c r="B62" s="212" t="n"/>
-      <c r="C62" s="212" t="n"/>
+      <c r="C62" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D62" s="25" t="n"/>
-      <c r="E62" s="26" t="n"/>
+      <c r="E62" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F62" s="27" t="n"/>
       <c r="G62" s="210" t="n"/>
       <c r="H62" s="320" t="n"/>
@@ -32355,7 +33159,11 @@
       <c r="N62" s="210" t="n"/>
       <c r="O62" s="320" t="n"/>
       <c r="P62" s="319" t="n"/>
-      <c r="Q62" s="31" t="n"/>
+      <c r="Q62" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R62" s="32" t="n"/>
       <c r="S62" s="32" t="n"/>
       <c r="T62" s="32" t="n"/>
@@ -32373,11 +33181,23 @@
       <c r="AF62" s="33" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="24" t="n"/>
+      <c r="A63" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
       <c r="B63" s="212" t="n"/>
-      <c r="C63" s="212" t="n"/>
+      <c r="C63" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D63" s="25" t="n"/>
-      <c r="E63" s="26" t="n"/>
+      <c r="E63" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F63" s="27" t="n"/>
       <c r="G63" s="210" t="n"/>
       <c r="H63" s="320" t="n"/>
@@ -32389,7 +33209,11 @@
       <c r="N63" s="210" t="n"/>
       <c r="O63" s="320" t="n"/>
       <c r="P63" s="319" t="n"/>
-      <c r="Q63" s="31" t="n"/>
+      <c r="Q63" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R63" s="32" t="n"/>
       <c r="S63" s="32" t="n"/>
       <c r="T63" s="32" t="n"/>
@@ -32407,11 +33231,23 @@
       <c r="AF63" s="33" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" s="24" t="n"/>
+      <c r="A64" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-09</t>
+        </is>
+      </c>
       <c r="B64" s="212" t="n"/>
-      <c r="C64" s="212" t="n"/>
+      <c r="C64" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D64" s="25" t="n"/>
-      <c r="E64" s="26" t="n"/>
+      <c r="E64" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F64" s="27" t="n"/>
       <c r="G64" s="210" t="n"/>
       <c r="H64" s="320" t="n"/>
@@ -32423,7 +33259,11 @@
       <c r="N64" s="210" t="n"/>
       <c r="O64" s="320" t="n"/>
       <c r="P64" s="319" t="n"/>
-      <c r="Q64" s="31" t="n"/>
+      <c r="Q64" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R64" s="32" t="n"/>
       <c r="S64" s="32" t="n"/>
       <c r="T64" s="32" t="n"/>
@@ -32441,11 +33281,23 @@
       <c r="AF64" s="33" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="24" t="n"/>
+      <c r="A65" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
       <c r="B65" s="212" t="n"/>
-      <c r="C65" s="212" t="n"/>
+      <c r="C65" s="212" t="inlineStr">
+        <is>
+          <t>6.25</t>
+        </is>
+      </c>
       <c r="D65" s="25" t="n"/>
-      <c r="E65" s="26" t="n"/>
+      <c r="E65" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F65" s="27" t="n"/>
       <c r="G65" s="210" t="n"/>
       <c r="H65" s="320" t="n"/>
@@ -32457,7 +33309,11 @@
       <c r="N65" s="210" t="n"/>
       <c r="O65" s="320" t="n"/>
       <c r="P65" s="319" t="n"/>
-      <c r="Q65" s="31" t="n"/>
+      <c r="Q65" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 14:30-20:45</t>
+        </is>
+      </c>
       <c r="R65" s="32" t="n"/>
       <c r="S65" s="32" t="n"/>
       <c r="T65" s="32" t="n"/>
@@ -33084,8 +33940,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="31.28515625" customWidth="1" min="1" max="1"/>
-    <col hidden="1" min="6" max="6"/>
-    <col hidden="1" min="9" max="9"/>
+    <col hidden="1" width="13" customWidth="1" min="6" max="6"/>
+    <col hidden="1" width="13" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -37505,11 +38361,23 @@
       <c r="AF58" s="33" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="24" t="n"/>
+      <c r="A59" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
       <c r="B59" s="212" t="n"/>
-      <c r="C59" s="212" t="n"/>
+      <c r="C59" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
       <c r="D59" s="25" t="n"/>
-      <c r="E59" s="26" t="n"/>
+      <c r="E59" s="26" t="inlineStr">
+        <is>
+          <t>US NCL</t>
+        </is>
+      </c>
       <c r="F59" s="27" t="n"/>
       <c r="G59" s="210" t="n"/>
       <c r="H59" s="320" t="n"/>
@@ -37521,7 +38389,11 @@
       <c r="N59" s="210" t="n"/>
       <c r="O59" s="320" t="n"/>
       <c r="P59" s="319" t="n"/>
-      <c r="Q59" s="31" t="n"/>
+      <c r="Q59" s="31" t="inlineStr">
+        <is>
+          <t>US NCL 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R59" s="32" t="n"/>
       <c r="S59" s="32" t="n"/>
       <c r="T59" s="32" t="n"/>
@@ -37539,11 +38411,23 @@
       <c r="AF59" s="33" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="24" t="n"/>
+      <c r="A60" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-03</t>
+        </is>
+      </c>
       <c r="B60" s="212" t="n"/>
-      <c r="C60" s="212" t="n"/>
+      <c r="C60" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
       <c r="D60" s="25" t="n"/>
-      <c r="E60" s="26" t="n"/>
+      <c r="E60" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F60" s="27" t="n"/>
       <c r="G60" s="210" t="n"/>
       <c r="H60" s="320" t="n"/>
@@ -37555,7 +38439,11 @@
       <c r="N60" s="210" t="n"/>
       <c r="O60" s="320" t="n"/>
       <c r="P60" s="319" t="n"/>
-      <c r="Q60" s="31" t="n"/>
+      <c r="Q60" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R60" s="32" t="n"/>
       <c r="S60" s="32" t="n"/>
       <c r="T60" s="32" t="n"/>
@@ -37573,11 +38461,23 @@
       <c r="AF60" s="33" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" s="24" t="n"/>
+      <c r="A61" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-12</t>
+        </is>
+      </c>
       <c r="B61" s="212" t="n"/>
-      <c r="C61" s="212" t="n"/>
+      <c r="C61" s="212" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
       <c r="D61" s="25" t="n"/>
-      <c r="E61" s="26" t="n"/>
+      <c r="E61" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F61" s="27" t="n"/>
       <c r="G61" s="210" t="n"/>
       <c r="H61" s="320" t="n"/>
@@ -37589,7 +38489,11 @@
       <c r="N61" s="210" t="n"/>
       <c r="O61" s="320" t="n"/>
       <c r="P61" s="319" t="n"/>
-      <c r="Q61" s="31" t="n"/>
+      <c r="Q61" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 13:30-13:44</t>
+        </is>
+      </c>
       <c r="R61" s="32" t="n"/>
       <c r="S61" s="32" t="n"/>
       <c r="T61" s="32" t="n"/>
@@ -37607,11 +38511,23 @@
       <c r="AF61" s="33" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" s="24" t="n"/>
+      <c r="A62" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-16</t>
+        </is>
+      </c>
       <c r="B62" s="212" t="n"/>
-      <c r="C62" s="212" t="n"/>
+      <c r="C62" s="212" t="inlineStr">
+        <is>
+          <t>4.50</t>
+        </is>
+      </c>
       <c r="D62" s="25" t="n"/>
-      <c r="E62" s="26" t="n"/>
+      <c r="E62" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F62" s="27" t="n"/>
       <c r="G62" s="210" t="n"/>
       <c r="H62" s="320" t="n"/>
@@ -37623,7 +38539,11 @@
       <c r="N62" s="210" t="n"/>
       <c r="O62" s="320" t="n"/>
       <c r="P62" s="319" t="n"/>
-      <c r="Q62" s="31" t="n"/>
+      <c r="Q62" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 13:30-18:00</t>
+        </is>
+      </c>
       <c r="R62" s="32" t="n"/>
       <c r="S62" s="32" t="n"/>
       <c r="T62" s="32" t="n"/>
@@ -40200,11 +41120,23 @@
       <c r="AF45" s="167" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="24" t="n"/>
+      <c r="A46" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B46" s="212" t="n"/>
-      <c r="C46" s="212" t="n"/>
+      <c r="C46" s="212" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
       <c r="D46" s="25" t="n"/>
-      <c r="E46" s="26" t="n"/>
+      <c r="E46" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F46" s="27" t="n"/>
       <c r="G46" s="210" t="n"/>
       <c r="H46" s="320" t="n"/>
@@ -40216,7 +41148,11 @@
       <c r="N46" s="210" t="n"/>
       <c r="O46" s="320" t="n"/>
       <c r="P46" s="319" t="n"/>
-      <c r="Q46" s="316" t="n"/>
+      <c r="Q46" s="316" t="inlineStr">
+        <is>
+          <t>US Tardy 11:45-13:18</t>
+        </is>
+      </c>
       <c r="R46" s="317" t="n"/>
       <c r="S46" s="317" t="n"/>
       <c r="T46" s="317" t="n"/>
@@ -40234,11 +41170,23 @@
       <c r="AF46" s="318" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="24" t="n"/>
+      <c r="A47" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
       <c r="B47" s="212" t="n"/>
-      <c r="C47" s="212" t="n"/>
+      <c r="C47" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D47" s="25" t="n"/>
-      <c r="E47" s="26" t="n"/>
+      <c r="E47" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F47" s="27" t="n"/>
       <c r="G47" s="210" t="n"/>
       <c r="H47" s="320" t="n"/>
@@ -40250,7 +41198,11 @@
       <c r="N47" s="210" t="n"/>
       <c r="O47" s="320" t="n"/>
       <c r="P47" s="319" t="n"/>
-      <c r="Q47" s="153" t="n"/>
+      <c r="Q47" s="153" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 11:45-22:00</t>
+        </is>
+      </c>
       <c r="R47" s="320" t="n"/>
       <c r="S47" s="320" t="n"/>
       <c r="T47" s="320" t="n"/>
@@ -40268,11 +41220,23 @@
       <c r="AF47" s="319" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="24" t="n"/>
+      <c r="A48" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-14</t>
+        </is>
+      </c>
       <c r="B48" s="212" t="n"/>
-      <c r="C48" s="212" t="n"/>
+      <c r="C48" s="212" t="inlineStr">
+        <is>
+          <t>4.85</t>
+        </is>
+      </c>
       <c r="D48" s="25" t="n"/>
-      <c r="E48" s="26" t="n"/>
+      <c r="E48" s="26" t="inlineStr">
+        <is>
+          <t>US Partial</t>
+        </is>
+      </c>
       <c r="F48" s="27" t="n"/>
       <c r="G48" s="210" t="n"/>
       <c r="H48" s="320" t="n"/>
@@ -40284,7 +41248,11 @@
       <c r="N48" s="210" t="n"/>
       <c r="O48" s="320" t="n"/>
       <c r="P48" s="319" t="n"/>
-      <c r="Q48" s="153" t="n"/>
+      <c r="Q48" s="153" t="inlineStr">
+        <is>
+          <t>US Partial 17:09-22:00</t>
+        </is>
+      </c>
       <c r="R48" s="320" t="n"/>
       <c r="S48" s="320" t="n"/>
       <c r="T48" s="320" t="n"/>
@@ -40302,11 +41270,23 @@
       <c r="AF48" s="319" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="24" t="n"/>
+      <c r="A49" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-14</t>
+        </is>
+      </c>
       <c r="B49" s="212" t="n"/>
-      <c r="C49" s="212" t="n"/>
+      <c r="C49" s="212" t="inlineStr">
+        <is>
+          <t>1.08</t>
+        </is>
+      </c>
       <c r="D49" s="25" t="n"/>
-      <c r="E49" s="26" t="n"/>
+      <c r="E49" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F49" s="27" t="n"/>
       <c r="G49" s="210" t="n"/>
       <c r="H49" s="320" t="n"/>
@@ -40318,7 +41298,11 @@
       <c r="N49" s="210" t="n"/>
       <c r="O49" s="320" t="n"/>
       <c r="P49" s="319" t="n"/>
-      <c r="Q49" s="153" t="n"/>
+      <c r="Q49" s="153" t="inlineStr">
+        <is>
+          <t>US Tardy 11:45-12:50</t>
+        </is>
+      </c>
       <c r="R49" s="320" t="n"/>
       <c r="S49" s="320" t="n"/>
       <c r="T49" s="320" t="n"/>
@@ -40336,11 +41320,23 @@
       <c r="AF49" s="319" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="24" t="n"/>
+      <c r="A50" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
       <c r="B50" s="212" t="n"/>
-      <c r="C50" s="212" t="n"/>
+      <c r="C50" s="212" t="inlineStr">
+        <is>
+          <t>3.20</t>
+        </is>
+      </c>
       <c r="D50" s="25" t="n"/>
-      <c r="E50" s="26" t="n"/>
+      <c r="E50" s="26" t="inlineStr">
+        <is>
+          <t>US Partial</t>
+        </is>
+      </c>
       <c r="F50" s="27" t="n"/>
       <c r="G50" s="210" t="n"/>
       <c r="H50" s="320" t="n"/>
@@ -40352,7 +41348,11 @@
       <c r="N50" s="210" t="n"/>
       <c r="O50" s="320" t="n"/>
       <c r="P50" s="319" t="n"/>
-      <c r="Q50" s="153" t="n"/>
+      <c r="Q50" s="153" t="inlineStr">
+        <is>
+          <t>US Partial 18:48-22:00</t>
+        </is>
+      </c>
       <c r="R50" s="320" t="n"/>
       <c r="S50" s="320" t="n"/>
       <c r="T50" s="320" t="n"/>
@@ -41507,7 +42507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK89"/>
+  <dimension ref="A1:AK95"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="Q82" sqref="Q82"/>
@@ -45329,6 +46329,138 @@
         </is>
       </c>
       <c r="Q89" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 09:00-19:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2023-12-16</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-09:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2023-12-23</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-09:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-10:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2024-01-06</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-09:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-01-13</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-09:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
+      <c r="Q95" t="inlineStr">
         <is>
           <t>US Absent Unplanned 09:00-19:15</t>
         </is>
@@ -45679,7 +46811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DL75"/>
+  <dimension ref="A1:DL77"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="Q51" sqref="Q51:AF178"/>
@@ -45688,8 +46820,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="31.28515625" customWidth="1" min="1" max="1"/>
-    <col hidden="1" min="6" max="6"/>
-    <col hidden="1" min="9" max="9"/>
+    <col hidden="1" width="13" customWidth="1" min="6" max="6"/>
+    <col hidden="1" width="13" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -50609,11 +51741,23 @@
       <c r="AF68" s="33" t="n"/>
     </row>
     <row r="69">
-      <c r="A69" s="24" t="n"/>
+      <c r="A69" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-15</t>
+        </is>
+      </c>
       <c r="B69" s="212" t="n"/>
-      <c r="C69" s="212" t="n"/>
+      <c r="C69" s="212" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
       <c r="D69" s="25" t="n"/>
-      <c r="E69" s="26" t="n"/>
+      <c r="E69" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F69" s="27" t="n"/>
       <c r="G69" s="210" t="n"/>
       <c r="H69" s="320" t="n"/>
@@ -50625,7 +51769,11 @@
       <c r="N69" s="210" t="n"/>
       <c r="O69" s="320" t="n"/>
       <c r="P69" s="319" t="n"/>
-      <c r="Q69" s="31" t="n"/>
+      <c r="Q69" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-11:12</t>
+        </is>
+      </c>
       <c r="R69" s="32" t="n"/>
       <c r="S69" s="32" t="n"/>
       <c r="T69" s="32" t="n"/>
@@ -50643,11 +51791,23 @@
       <c r="AF69" s="33" t="n"/>
     </row>
     <row r="70">
-      <c r="A70" s="24" t="n"/>
+      <c r="A70" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B70" s="212" t="n"/>
-      <c r="C70" s="212" t="n"/>
+      <c r="C70" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D70" s="25" t="n"/>
-      <c r="E70" s="26" t="n"/>
+      <c r="E70" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F70" s="27" t="n"/>
       <c r="G70" s="210" t="n"/>
       <c r="H70" s="320" t="n"/>
@@ -50659,7 +51819,11 @@
       <c r="N70" s="210" t="n"/>
       <c r="O70" s="320" t="n"/>
       <c r="P70" s="319" t="n"/>
-      <c r="Q70" s="31" t="n"/>
+      <c r="Q70" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:00-20:15</t>
+        </is>
+      </c>
       <c r="R70" s="32" t="n"/>
       <c r="S70" s="32" t="n"/>
       <c r="T70" s="32" t="n"/>
@@ -50677,11 +51841,23 @@
       <c r="AF70" s="33" t="n"/>
     </row>
     <row r="71">
-      <c r="A71" s="24" t="n"/>
+      <c r="A71" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-26</t>
+        </is>
+      </c>
       <c r="B71" s="212" t="n"/>
-      <c r="C71" s="212" t="n"/>
+      <c r="C71" s="212" t="inlineStr">
+        <is>
+          <t>8.97</t>
+        </is>
+      </c>
       <c r="D71" s="25" t="n"/>
-      <c r="E71" s="26" t="n"/>
+      <c r="E71" s="26" t="inlineStr">
+        <is>
+          <t>US Partial</t>
+        </is>
+      </c>
       <c r="F71" s="27" t="n"/>
       <c r="G71" s="210" t="n"/>
       <c r="H71" s="320" t="n"/>
@@ -50693,7 +51869,11 @@
       <c r="N71" s="210" t="n"/>
       <c r="O71" s="320" t="n"/>
       <c r="P71" s="319" t="n"/>
-      <c r="Q71" s="31" t="n"/>
+      <c r="Q71" s="31" t="inlineStr">
+        <is>
+          <t>US Partial 11:17-20:15</t>
+        </is>
+      </c>
       <c r="R71" s="32" t="n"/>
       <c r="S71" s="32" t="n"/>
       <c r="T71" s="32" t="n"/>
@@ -50711,11 +51891,23 @@
       <c r="AF71" s="33" t="n"/>
     </row>
     <row r="72">
-      <c r="A72" s="24" t="n"/>
+      <c r="A72" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-30</t>
+        </is>
+      </c>
       <c r="B72" s="212" t="n"/>
-      <c r="C72" s="212" t="n"/>
+      <c r="C72" s="212" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
       <c r="D72" s="25" t="n"/>
-      <c r="E72" s="26" t="n"/>
+      <c r="E72" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F72" s="27" t="n"/>
       <c r="G72" s="210" t="n"/>
       <c r="H72" s="320" t="n"/>
@@ -50727,7 +51919,11 @@
       <c r="N72" s="210" t="n"/>
       <c r="O72" s="320" t="n"/>
       <c r="P72" s="319" t="n"/>
-      <c r="Q72" s="31" t="n"/>
+      <c r="Q72" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-10:36</t>
+        </is>
+      </c>
       <c r="R72" s="32" t="n"/>
       <c r="S72" s="32" t="n"/>
       <c r="T72" s="32" t="n"/>
@@ -50745,11 +51941,23 @@
       <c r="AF72" s="33" t="n"/>
     </row>
     <row r="73">
-      <c r="A73" s="24" t="n"/>
+      <c r="A73" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
       <c r="B73" s="212" t="n"/>
-      <c r="C73" s="212" t="n"/>
+      <c r="C73" s="212" t="inlineStr">
+        <is>
+          <t>5.33</t>
+        </is>
+      </c>
       <c r="D73" s="25" t="n"/>
-      <c r="E73" s="26" t="n"/>
+      <c r="E73" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F73" s="27" t="n"/>
       <c r="G73" s="210" t="n"/>
       <c r="H73" s="320" t="n"/>
@@ -50761,7 +51969,11 @@
       <c r="N73" s="210" t="n"/>
       <c r="O73" s="320" t="n"/>
       <c r="P73" s="319" t="n"/>
-      <c r="Q73" s="31" t="n"/>
+      <c r="Q73" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-15:20</t>
+        </is>
+      </c>
       <c r="R73" s="32" t="n"/>
       <c r="S73" s="32" t="n"/>
       <c r="T73" s="32" t="n"/>
@@ -50779,11 +51991,23 @@
       <c r="AF73" s="33" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" s="24" t="n"/>
+      <c r="A74" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-02</t>
+        </is>
+      </c>
       <c r="B74" s="212" t="n"/>
-      <c r="C74" s="212" t="n"/>
+      <c r="C74" s="212" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
       <c r="D74" s="25" t="n"/>
-      <c r="E74" s="26" t="n"/>
+      <c r="E74" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F74" s="27" t="n"/>
       <c r="G74" s="210" t="n"/>
       <c r="H74" s="320" t="n"/>
@@ -50795,7 +52019,11 @@
       <c r="N74" s="210" t="n"/>
       <c r="O74" s="320" t="n"/>
       <c r="P74" s="319" t="n"/>
-      <c r="Q74" s="31" t="n"/>
+      <c r="Q74" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-10:22</t>
+        </is>
+      </c>
       <c r="R74" s="32" t="n"/>
       <c r="S74" s="32" t="n"/>
       <c r="T74" s="32" t="n"/>
@@ -50813,11 +52041,23 @@
       <c r="AF74" s="33" t="n"/>
     </row>
     <row r="75">
-      <c r="A75" s="24" t="n"/>
+      <c r="A75" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-05</t>
+        </is>
+      </c>
       <c r="B75" s="212" t="n"/>
-      <c r="C75" s="212" t="n"/>
+      <c r="C75" s="212" t="inlineStr">
+        <is>
+          <t>3.92</t>
+        </is>
+      </c>
       <c r="D75" s="25" t="n"/>
-      <c r="E75" s="26" t="n"/>
+      <c r="E75" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F75" s="27" t="n"/>
       <c r="G75" s="210" t="n"/>
       <c r="H75" s="320" t="n"/>
@@ -50829,7 +52069,11 @@
       <c r="N75" s="210" t="n"/>
       <c r="O75" s="320" t="n"/>
       <c r="P75" s="319" t="n"/>
-      <c r="Q75" s="31" t="n"/>
+      <c r="Q75" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-13:55</t>
+        </is>
+      </c>
       <c r="R75" s="32" t="n"/>
       <c r="S75" s="32" t="n"/>
       <c r="T75" s="32" t="n"/>
@@ -50845,6 +52089,50 @@
       <c r="AD75" s="32" t="n"/>
       <c r="AE75" s="32" t="n"/>
       <c r="AF75" s="33" t="n"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:00-20:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:00-20:15</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="206">

</xml_diff>

<commit_message>
January 27, 2024 12:58pm
</commit_message>
<xml_diff>
--- a/AttendanceTracker.xlsx
+++ b/AttendanceTracker.xlsx
@@ -4193,11 +4193,23 @@
       <c r="AF42" s="147" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="24" t="n"/>
+      <c r="A43" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-22</t>
+        </is>
+      </c>
       <c r="B43" s="212" t="n"/>
-      <c r="C43" s="212" t="n"/>
+      <c r="C43" s="212" t="inlineStr">
+        <is>
+          <t>0.95</t>
+        </is>
+      </c>
       <c r="D43" s="25" t="n"/>
-      <c r="E43" s="26" t="n"/>
+      <c r="E43" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F43" s="27" t="n"/>
       <c r="G43" s="210" t="n"/>
       <c r="H43" s="320" t="n"/>
@@ -4209,7 +4221,11 @@
       <c r="N43" s="210" t="n"/>
       <c r="O43" s="320" t="n"/>
       <c r="P43" s="319" t="n"/>
-      <c r="Q43" s="148" t="n"/>
+      <c r="Q43" s="148" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-09:57</t>
+        </is>
+      </c>
       <c r="R43" s="149" t="n"/>
       <c r="S43" s="149" t="n"/>
       <c r="T43" s="149" t="n"/>
@@ -4227,11 +4243,23 @@
       <c r="AF43" s="150" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="24" t="n"/>
+      <c r="A44" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
       <c r="B44" s="212" t="n"/>
-      <c r="C44" s="212" t="n"/>
+      <c r="C44" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D44" s="25" t="n"/>
-      <c r="E44" s="26" t="n"/>
+      <c r="E44" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F44" s="27" t="n"/>
       <c r="G44" s="210" t="n"/>
       <c r="H44" s="320" t="n"/>
@@ -4243,7 +4271,11 @@
       <c r="N44" s="210" t="n"/>
       <c r="O44" s="320" t="n"/>
       <c r="P44" s="319" t="n"/>
-      <c r="Q44" s="146" t="n"/>
+      <c r="Q44" s="146" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 09:00-19:15</t>
+        </is>
+      </c>
       <c r="R44" s="40" t="n"/>
       <c r="S44" s="40" t="n"/>
       <c r="T44" s="40" t="n"/>
@@ -5575,7 +5607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
@@ -6313,6 +6345,94 @@
         </is>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>US Tardy 11:30-11:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-01-05</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>10.50</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 11:30-22:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-01-14</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>US Tardy 11:30-12:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>1.08</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>US Tardy 11:30-12:35</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6324,7 +6444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG176"/>
+  <dimension ref="A1:AG178"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="J85" sqref="J85:M85"/>
@@ -14650,10 +14770,22 @@
       <c r="AF153" s="319" t="n"/>
     </row>
     <row r="154">
-      <c r="A154" s="24" t="n"/>
+      <c r="A154" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-15</t>
+        </is>
+      </c>
       <c r="B154" s="212" t="inlineStr"/>
-      <c r="C154" s="212" t="n"/>
-      <c r="D154" s="212" t="n"/>
+      <c r="C154" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D154" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E154" s="320" t="n"/>
       <c r="F154" s="319" t="n"/>
       <c r="G154" s="210" t="n"/>
@@ -14666,7 +14798,11 @@
       <c r="N154" s="210" t="n"/>
       <c r="O154" s="320" t="n"/>
       <c r="P154" s="319" t="n"/>
-      <c r="Q154" s="253" t="n"/>
+      <c r="Q154" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R154" s="320" t="n"/>
       <c r="S154" s="320" t="n"/>
       <c r="T154" s="320" t="n"/>
@@ -14684,10 +14820,22 @@
       <c r="AF154" s="319" t="n"/>
     </row>
     <row r="155">
-      <c r="A155" s="24" t="n"/>
+      <c r="A155" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-16</t>
+        </is>
+      </c>
       <c r="B155" s="212" t="inlineStr"/>
-      <c r="C155" s="212" t="n"/>
-      <c r="D155" s="212" t="n"/>
+      <c r="C155" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D155" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E155" s="320" t="n"/>
       <c r="F155" s="319" t="n"/>
       <c r="G155" s="210" t="n"/>
@@ -14700,7 +14848,11 @@
       <c r="N155" s="210" t="n"/>
       <c r="O155" s="320" t="n"/>
       <c r="P155" s="319" t="n"/>
-      <c r="Q155" s="253" t="n"/>
+      <c r="Q155" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R155" s="320" t="n"/>
       <c r="S155" s="320" t="n"/>
       <c r="T155" s="320" t="n"/>
@@ -14718,10 +14870,22 @@
       <c r="AF155" s="319" t="n"/>
     </row>
     <row r="156">
-      <c r="A156" s="24" t="n"/>
+      <c r="A156" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B156" s="212" t="inlineStr"/>
-      <c r="C156" s="212" t="n"/>
-      <c r="D156" s="212" t="n"/>
+      <c r="C156" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="D156" s="212" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
       <c r="E156" s="320" t="n"/>
       <c r="F156" s="319" t="n"/>
       <c r="G156" s="210" t="n"/>
@@ -14734,7 +14898,11 @@
       <c r="N156" s="210" t="n"/>
       <c r="O156" s="320" t="n"/>
       <c r="P156" s="319" t="n"/>
-      <c r="Q156" s="253" t="n"/>
+      <c r="Q156" s="253" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R156" s="320" t="n"/>
       <c r="S156" s="320" t="n"/>
       <c r="T156" s="320" t="n"/>
@@ -14752,64 +14920,488 @@
       <c r="AF156" s="319" t="n"/>
     </row>
     <row r="157">
-      <c r="A157" s="41" t="n"/>
+      <c r="A157" s="41" t="inlineStr">
+        <is>
+          <t>2023-12-19</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q157" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="158">
-      <c r="A158" s="41" t="n"/>
+      <c r="A158" s="41" t="inlineStr">
+        <is>
+          <t>2023-12-20</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q158" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="159">
-      <c r="A159" s="41" t="n"/>
+      <c r="A159" s="41" t="inlineStr">
+        <is>
+          <t>2023-12-22</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q159" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="160">
-      <c r="A160" s="41" t="n"/>
+      <c r="A160" s="41" t="inlineStr">
+        <is>
+          <t>2023-12-23</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="161">
-      <c r="A161" s="41" t="n"/>
+      <c r="A161" s="41" t="inlineStr">
+        <is>
+          <t>2023-12-25</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q161" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="162">
-      <c r="A162" s="41" t="n"/>
+      <c r="A162" s="41" t="inlineStr">
+        <is>
+          <t>2023-12-26</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="163">
-      <c r="A163" s="41" t="n"/>
+      <c r="A163" s="41" t="inlineStr">
+        <is>
+          <t>2023-12-27</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="164">
-      <c r="A164" s="41" t="n"/>
+      <c r="A164" s="41" t="inlineStr">
+        <is>
+          <t>2023-12-29</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q164" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="165">
-      <c r="A165" s="41" t="n"/>
+      <c r="A165" s="41" t="inlineStr">
+        <is>
+          <t>2023-12-30</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q165" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="166">
-      <c r="A166" s="41" t="n"/>
+      <c r="A166" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="167">
-      <c r="A167" s="41" t="n"/>
+      <c r="A167" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-02</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="168">
-      <c r="A168" s="41" t="n"/>
+      <c r="A168" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-03</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="169">
-      <c r="A169" s="41" t="n"/>
+      <c r="A169" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-05</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q169" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="170">
-      <c r="A170" s="41" t="n"/>
+      <c r="A170" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-06</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q170" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="171">
-      <c r="A171" s="41" t="n"/>
+      <c r="A171" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q171" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="172">
-      <c r="A172" s="41" t="n"/>
+      <c r="A172" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-09</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q172" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="173">
-      <c r="A173" s="41" t="n"/>
+      <c r="A173" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-10</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q173" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="174">
-      <c r="A174" s="41" t="n"/>
+      <c r="A174" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-12</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q174" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="175">
-      <c r="A175" s="41" t="n"/>
+      <c r="A175" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-13</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q175" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
     </row>
     <row r="176">
-      <c r="A176" s="41" t="n"/>
+      <c r="A176" s="41" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q176" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2024-01-16</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q177" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-22:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>6.50</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>US LOA</t>
+        </is>
+      </c>
+      <c r="Q178" t="inlineStr">
+        <is>
+          <t>US LOA 13:30-20:00</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="670">
@@ -17778,11 +18370,23 @@
       <c r="AF51" s="33" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="24" t="n"/>
+      <c r="A52" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-16</t>
+        </is>
+      </c>
       <c r="B52" s="212" t="n"/>
-      <c r="C52" s="212" t="n"/>
+      <c r="C52" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D52" s="25" t="n"/>
-      <c r="E52" s="26" t="n"/>
+      <c r="E52" s="26" t="inlineStr">
+        <is>
+          <t>US Bereavement</t>
+        </is>
+      </c>
       <c r="F52" s="27" t="n"/>
       <c r="G52" s="210" t="n"/>
       <c r="H52" s="320" t="n"/>
@@ -17794,7 +18398,11 @@
       <c r="N52" s="210" t="n"/>
       <c r="O52" s="320" t="n"/>
       <c r="P52" s="319" t="n"/>
-      <c r="Q52" s="31" t="n"/>
+      <c r="Q52" s="31" t="inlineStr">
+        <is>
+          <t>US Bereavement 11:45-22:00</t>
+        </is>
+      </c>
       <c r="R52" s="32" t="n"/>
       <c r="S52" s="32" t="n"/>
       <c r="T52" s="32" t="n"/>
@@ -17812,11 +18420,23 @@
       <c r="AF52" s="33" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="24" t="n"/>
+      <c r="A53" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B53" s="212" t="n"/>
-      <c r="C53" s="212" t="n"/>
+      <c r="C53" s="212" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
       <c r="D53" s="25" t="n"/>
-      <c r="E53" s="26" t="n"/>
+      <c r="E53" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F53" s="27" t="n"/>
       <c r="G53" s="210" t="n"/>
       <c r="H53" s="320" t="n"/>
@@ -17828,7 +18448,11 @@
       <c r="N53" s="210" t="n"/>
       <c r="O53" s="320" t="n"/>
       <c r="P53" s="319" t="n"/>
-      <c r="Q53" s="31" t="n"/>
+      <c r="Q53" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 14:45-15:15</t>
+        </is>
+      </c>
       <c r="R53" s="32" t="n"/>
       <c r="S53" s="32" t="n"/>
       <c r="T53" s="32" t="n"/>
@@ -17846,11 +18470,23 @@
       <c r="AF53" s="33" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="24" t="n"/>
+      <c r="A54" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-23</t>
+        </is>
+      </c>
       <c r="B54" s="212" t="n"/>
-      <c r="C54" s="212" t="n"/>
+      <c r="C54" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D54" s="25" t="n"/>
-      <c r="E54" s="26" t="n"/>
+      <c r="E54" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F54" s="27" t="n"/>
       <c r="G54" s="210" t="n"/>
       <c r="H54" s="320" t="n"/>
@@ -17862,7 +18498,11 @@
       <c r="N54" s="210" t="n"/>
       <c r="O54" s="320" t="n"/>
       <c r="P54" s="319" t="n"/>
-      <c r="Q54" s="31" t="n"/>
+      <c r="Q54" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 11:45-22:00</t>
+        </is>
+      </c>
       <c r="R54" s="32" t="n"/>
       <c r="S54" s="32" t="n"/>
       <c r="T54" s="32" t="n"/>
@@ -17880,11 +18520,23 @@
       <c r="AF54" s="33" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="24" t="n"/>
+      <c r="A55" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-30</t>
+        </is>
+      </c>
       <c r="B55" s="212" t="n"/>
-      <c r="C55" s="212" t="n"/>
+      <c r="C55" s="212" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
       <c r="D55" s="25" t="n"/>
-      <c r="E55" s="26" t="n"/>
+      <c r="E55" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F55" s="27" t="n"/>
       <c r="G55" s="210" t="n"/>
       <c r="H55" s="320" t="n"/>
@@ -17896,7 +18548,11 @@
       <c r="N55" s="210" t="n"/>
       <c r="O55" s="320" t="n"/>
       <c r="P55" s="319" t="n"/>
-      <c r="Q55" s="31" t="n"/>
+      <c r="Q55" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 11:45-11:55</t>
+        </is>
+      </c>
       <c r="R55" s="32" t="n"/>
       <c r="S55" s="32" t="n"/>
       <c r="T55" s="32" t="n"/>
@@ -17914,11 +18570,23 @@
       <c r="AF55" s="33" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="24" t="n"/>
+      <c r="A56" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-10</t>
+        </is>
+      </c>
       <c r="B56" s="212" t="n"/>
-      <c r="C56" s="212" t="n"/>
+      <c r="C56" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D56" s="25" t="n"/>
-      <c r="E56" s="26" t="n"/>
+      <c r="E56" s="26" t="inlineStr">
+        <is>
+          <t>US NCL</t>
+        </is>
+      </c>
       <c r="F56" s="27" t="n"/>
       <c r="G56" s="210" t="n"/>
       <c r="H56" s="320" t="n"/>
@@ -17930,7 +18598,11 @@
       <c r="N56" s="210" t="n"/>
       <c r="O56" s="320" t="n"/>
       <c r="P56" s="319" t="n"/>
-      <c r="Q56" s="31" t="n"/>
+      <c r="Q56" s="31" t="inlineStr">
+        <is>
+          <t>US NCL 11:45-22:00</t>
+        </is>
+      </c>
       <c r="R56" s="32" t="n"/>
       <c r="S56" s="32" t="n"/>
       <c r="T56" s="32" t="n"/>
@@ -17948,11 +18620,23 @@
       <c r="AF56" s="33" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="24" t="n"/>
+      <c r="A57" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-13</t>
+        </is>
+      </c>
       <c r="B57" s="212" t="n"/>
-      <c r="C57" s="212" t="n"/>
+      <c r="C57" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D57" s="25" t="n"/>
-      <c r="E57" s="26" t="n"/>
+      <c r="E57" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F57" s="27" t="n"/>
       <c r="G57" s="210" t="n"/>
       <c r="H57" s="320" t="n"/>
@@ -17964,7 +18648,11 @@
       <c r="N57" s="210" t="n"/>
       <c r="O57" s="320" t="n"/>
       <c r="P57" s="319" t="n"/>
-      <c r="Q57" s="31" t="n"/>
+      <c r="Q57" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 11:45-22:00</t>
+        </is>
+      </c>
       <c r="R57" s="32" t="n"/>
       <c r="S57" s="32" t="n"/>
       <c r="T57" s="32" t="n"/>
@@ -22131,11 +22819,23 @@
       <c r="AF54" s="232" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="24" t="n"/>
+      <c r="A55" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-16</t>
+        </is>
+      </c>
       <c r="B55" s="212" t="n"/>
-      <c r="C55" s="212" t="n"/>
+      <c r="C55" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
       <c r="D55" s="212" t="n"/>
-      <c r="E55" s="212" t="n"/>
+      <c r="E55" s="212" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F55" s="212" t="n"/>
       <c r="G55" s="210" t="n"/>
       <c r="H55" s="320" t="n"/>
@@ -22147,7 +22847,11 @@
       <c r="N55" s="210" t="n"/>
       <c r="O55" s="320" t="n"/>
       <c r="P55" s="319" t="n"/>
-      <c r="Q55" s="232" t="n"/>
+      <c r="Q55" s="232" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R55" s="232" t="n"/>
       <c r="S55" s="232" t="n"/>
       <c r="T55" s="232" t="n"/>
@@ -22165,11 +22869,23 @@
       <c r="AF55" s="232" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="24" t="n"/>
+      <c r="A56" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-20</t>
+        </is>
+      </c>
       <c r="B56" s="212" t="n"/>
-      <c r="C56" s="212" t="n"/>
+      <c r="C56" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
       <c r="D56" s="212" t="n"/>
-      <c r="E56" s="212" t="n"/>
+      <c r="E56" s="212" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F56" s="212" t="n"/>
       <c r="G56" s="210" t="n"/>
       <c r="H56" s="320" t="n"/>
@@ -22181,7 +22897,11 @@
       <c r="N56" s="210" t="n"/>
       <c r="O56" s="320" t="n"/>
       <c r="P56" s="319" t="n"/>
-      <c r="Q56" s="264" t="n"/>
+      <c r="Q56" s="264" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R56" s="264" t="n"/>
       <c r="S56" s="264" t="n"/>
       <c r="T56" s="264" t="n"/>
@@ -22199,11 +22919,23 @@
       <c r="AF56" s="264" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="24" t="n"/>
+      <c r="A57" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
       <c r="B57" s="212" t="n"/>
-      <c r="C57" s="212" t="n"/>
+      <c r="C57" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
       <c r="D57" s="212" t="n"/>
-      <c r="E57" s="212" t="n"/>
+      <c r="E57" s="212" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F57" s="212" t="n"/>
       <c r="G57" s="210" t="n"/>
       <c r="H57" s="320" t="n"/>
@@ -22215,7 +22947,11 @@
       <c r="N57" s="210" t="n"/>
       <c r="O57" s="320" t="n"/>
       <c r="P57" s="319" t="n"/>
-      <c r="Q57" s="253" t="n"/>
+      <c r="Q57" s="253" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R57" s="253" t="n"/>
       <c r="S57" s="253" t="n"/>
       <c r="T57" s="253" t="n"/>
@@ -27780,11 +28516,23 @@
       <c r="AF41" s="152" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="24" t="n"/>
+      <c r="A42" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-16</t>
+        </is>
+      </c>
       <c r="B42" s="212" t="n"/>
-      <c r="C42" s="212" t="n"/>
+      <c r="C42" s="212" t="inlineStr">
+        <is>
+          <t>6.50</t>
+        </is>
+      </c>
       <c r="D42" s="25" t="n"/>
-      <c r="E42" s="26" t="n"/>
+      <c r="E42" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F42" s="27" t="n"/>
       <c r="G42" s="210" t="n"/>
       <c r="H42" s="320" t="n"/>
@@ -27796,7 +28544,11 @@
       <c r="N42" s="257" t="n"/>
       <c r="O42" s="320" t="n"/>
       <c r="P42" s="320" t="n"/>
-      <c r="Q42" s="232" t="n"/>
+      <c r="Q42" s="232" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 12:00-18:30</t>
+        </is>
+      </c>
       <c r="R42" s="232" t="n"/>
       <c r="S42" s="232" t="n"/>
       <c r="T42" s="232" t="n"/>
@@ -27814,11 +28566,23 @@
       <c r="AF42" s="232" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="73" t="n"/>
+      <c r="A43" s="73" t="inlineStr">
+        <is>
+          <t>2023-12-30</t>
+        </is>
+      </c>
       <c r="B43" s="212" t="n"/>
-      <c r="C43" s="212" t="n"/>
+      <c r="C43" s="212" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
       <c r="D43" s="25" t="n"/>
-      <c r="E43" s="26" t="n"/>
+      <c r="E43" s="26" t="inlineStr">
+        <is>
+          <t>US NCL</t>
+        </is>
+      </c>
       <c r="F43" s="27" t="n"/>
       <c r="G43" s="257" t="n"/>
       <c r="H43" s="29" t="n"/>
@@ -27830,7 +28594,11 @@
       <c r="N43" s="257" t="n"/>
       <c r="O43" s="29" t="n"/>
       <c r="P43" s="29" t="n"/>
-      <c r="Q43" s="232" t="n"/>
+      <c r="Q43" s="232" t="inlineStr">
+        <is>
+          <t>US NCL 17:30-18:30</t>
+        </is>
+      </c>
       <c r="R43" s="232" t="n"/>
       <c r="S43" s="232" t="n"/>
       <c r="T43" s="232" t="n"/>
@@ -27848,11 +28616,23 @@
       <c r="AF43" s="232" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="24" t="n"/>
+      <c r="A44" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
       <c r="B44" s="212" t="n"/>
-      <c r="C44" s="212" t="n"/>
+      <c r="C44" s="212" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
       <c r="D44" s="25" t="n"/>
-      <c r="E44" s="26" t="n"/>
+      <c r="E44" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F44" s="27" t="n"/>
       <c r="G44" s="210" t="n"/>
       <c r="H44" s="320" t="n"/>
@@ -27864,7 +28644,11 @@
       <c r="N44" s="257" t="n"/>
       <c r="O44" s="320" t="n"/>
       <c r="P44" s="320" t="n"/>
-      <c r="Q44" s="232" t="n"/>
+      <c r="Q44" s="232" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-10:12</t>
+        </is>
+      </c>
       <c r="R44" s="232" t="n"/>
       <c r="S44" s="232" t="n"/>
       <c r="T44" s="232" t="n"/>
@@ -33331,11 +34115,23 @@
       <c r="AF65" s="33" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="24" t="n"/>
+      <c r="A66" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-17</t>
+        </is>
+      </c>
       <c r="B66" s="212" t="n"/>
-      <c r="C66" s="212" t="n"/>
+      <c r="C66" s="212" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
       <c r="D66" s="25" t="n"/>
-      <c r="E66" s="26" t="n"/>
+      <c r="E66" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F66" s="27" t="n"/>
       <c r="G66" s="210" t="n"/>
       <c r="H66" s="320" t="n"/>
@@ -33347,7 +34143,11 @@
       <c r="N66" s="210" t="n"/>
       <c r="O66" s="320" t="n"/>
       <c r="P66" s="319" t="n"/>
-      <c r="Q66" s="31" t="n"/>
+      <c r="Q66" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 10:30-11:34</t>
+        </is>
+      </c>
       <c r="R66" s="32" t="n"/>
       <c r="S66" s="32" t="n"/>
       <c r="T66" s="32" t="n"/>
@@ -33365,11 +34165,23 @@
       <c r="AF66" s="33" t="n"/>
     </row>
     <row r="67">
-      <c r="A67" s="24" t="n"/>
+      <c r="A67" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-19</t>
+        </is>
+      </c>
       <c r="B67" s="212" t="n"/>
-      <c r="C67" s="212" t="n"/>
+      <c r="C67" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D67" s="25" t="n"/>
-      <c r="E67" s="26" t="n"/>
+      <c r="E67" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F67" s="27" t="n"/>
       <c r="G67" s="210" t="n"/>
       <c r="H67" s="320" t="n"/>
@@ -33381,7 +34193,11 @@
       <c r="N67" s="210" t="n"/>
       <c r="O67" s="320" t="n"/>
       <c r="P67" s="319" t="n"/>
-      <c r="Q67" s="31" t="n"/>
+      <c r="Q67" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R67" s="32" t="n"/>
       <c r="S67" s="32" t="n"/>
       <c r="T67" s="32" t="n"/>
@@ -33399,11 +34215,23 @@
       <c r="AF67" s="33" t="n"/>
     </row>
     <row r="68">
-      <c r="A68" s="24" t="n"/>
+      <c r="A68" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-26</t>
+        </is>
+      </c>
       <c r="B68" s="212" t="n"/>
-      <c r="C68" s="212" t="n"/>
+      <c r="C68" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D68" s="25" t="n"/>
-      <c r="E68" s="26" t="n"/>
+      <c r="E68" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F68" s="27" t="n"/>
       <c r="G68" s="210" t="n"/>
       <c r="H68" s="320" t="n"/>
@@ -33415,7 +34243,11 @@
       <c r="N68" s="210" t="n"/>
       <c r="O68" s="320" t="n"/>
       <c r="P68" s="319" t="n"/>
-      <c r="Q68" s="31" t="n"/>
+      <c r="Q68" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R68" s="32" t="n"/>
       <c r="S68" s="32" t="n"/>
       <c r="T68" s="32" t="n"/>
@@ -33433,11 +34265,23 @@
       <c r="AF68" s="33" t="n"/>
     </row>
     <row r="69">
-      <c r="A69" s="24" t="n"/>
+      <c r="A69" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-29</t>
+        </is>
+      </c>
       <c r="B69" s="212" t="n"/>
-      <c r="C69" s="212" t="n"/>
+      <c r="C69" s="212" t="inlineStr">
+        <is>
+          <t>3.67</t>
+        </is>
+      </c>
       <c r="D69" s="25" t="n"/>
-      <c r="E69" s="26" t="n"/>
+      <c r="E69" s="26" t="inlineStr">
+        <is>
+          <t>US Partial</t>
+        </is>
+      </c>
       <c r="F69" s="27" t="n"/>
       <c r="G69" s="210" t="n"/>
       <c r="H69" s="320" t="n"/>
@@ -33449,7 +34293,11 @@
       <c r="N69" s="210" t="n"/>
       <c r="O69" s="320" t="n"/>
       <c r="P69" s="319" t="n"/>
-      <c r="Q69" s="31" t="n"/>
+      <c r="Q69" s="31" t="inlineStr">
+        <is>
+          <t>US Partial 17:05-20:45</t>
+        </is>
+      </c>
       <c r="R69" s="32" t="n"/>
       <c r="S69" s="32" t="n"/>
       <c r="T69" s="32" t="n"/>
@@ -33467,11 +34315,23 @@
       <c r="AF69" s="33" t="n"/>
     </row>
     <row r="70">
-      <c r="A70" s="24" t="n"/>
+      <c r="A70" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
       <c r="B70" s="212" t="n"/>
-      <c r="C70" s="212" t="n"/>
+      <c r="C70" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D70" s="25" t="n"/>
-      <c r="E70" s="26" t="n"/>
+      <c r="E70" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F70" s="27" t="n"/>
       <c r="G70" s="210" t="n"/>
       <c r="H70" s="320" t="n"/>
@@ -33483,7 +34343,11 @@
       <c r="N70" s="210" t="n"/>
       <c r="O70" s="320" t="n"/>
       <c r="P70" s="319" t="n"/>
-      <c r="Q70" s="31" t="n"/>
+      <c r="Q70" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R70" s="32" t="n"/>
       <c r="S70" s="32" t="n"/>
       <c r="T70" s="32" t="n"/>
@@ -33501,11 +34365,23 @@
       <c r="AF70" s="33" t="n"/>
     </row>
     <row r="71">
-      <c r="A71" s="24" t="n"/>
+      <c r="A71" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-02</t>
+        </is>
+      </c>
       <c r="B71" s="212" t="n"/>
-      <c r="C71" s="212" t="n"/>
+      <c r="C71" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D71" s="25" t="n"/>
-      <c r="E71" s="26" t="n"/>
+      <c r="E71" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F71" s="27" t="n"/>
       <c r="G71" s="210" t="n"/>
       <c r="H71" s="320" t="n"/>
@@ -33517,7 +34393,11 @@
       <c r="N71" s="210" t="n"/>
       <c r="O71" s="320" t="n"/>
       <c r="P71" s="319" t="n"/>
-      <c r="Q71" s="31" t="n"/>
+      <c r="Q71" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R71" s="32" t="n"/>
       <c r="S71" s="32" t="n"/>
       <c r="T71" s="32" t="n"/>
@@ -33535,11 +34415,23 @@
       <c r="AF71" s="33" t="n"/>
     </row>
     <row r="72">
-      <c r="A72" s="24" t="n"/>
+      <c r="A72" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
       <c r="B72" s="212" t="n"/>
-      <c r="C72" s="212" t="n"/>
+      <c r="C72" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D72" s="25" t="n"/>
-      <c r="E72" s="26" t="n"/>
+      <c r="E72" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F72" s="27" t="n"/>
       <c r="G72" s="210" t="n"/>
       <c r="H72" s="320" t="n"/>
@@ -33551,7 +34443,11 @@
       <c r="N72" s="210" t="n"/>
       <c r="O72" s="320" t="n"/>
       <c r="P72" s="319" t="n"/>
-      <c r="Q72" s="31" t="n"/>
+      <c r="Q72" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R72" s="32" t="n"/>
       <c r="S72" s="32" t="n"/>
       <c r="T72" s="32" t="n"/>
@@ -33569,11 +34465,23 @@
       <c r="AF72" s="33" t="n"/>
     </row>
     <row r="73">
-      <c r="A73" s="24" t="n"/>
+      <c r="A73" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-09</t>
+        </is>
+      </c>
       <c r="B73" s="212" t="n"/>
-      <c r="C73" s="212" t="n"/>
+      <c r="C73" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D73" s="25" t="n"/>
-      <c r="E73" s="26" t="n"/>
+      <c r="E73" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F73" s="27" t="n"/>
       <c r="G73" s="210" t="n"/>
       <c r="H73" s="320" t="n"/>
@@ -33585,7 +34493,11 @@
       <c r="N73" s="210" t="n"/>
       <c r="O73" s="320" t="n"/>
       <c r="P73" s="319" t="n"/>
-      <c r="Q73" s="31" t="n"/>
+      <c r="Q73" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:30-20:45</t>
+        </is>
+      </c>
       <c r="R73" s="32" t="n"/>
       <c r="S73" s="32" t="n"/>
       <c r="T73" s="32" t="n"/>
@@ -33603,11 +34515,23 @@
       <c r="AF73" s="33" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" s="24" t="n"/>
+      <c r="A74" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
       <c r="B74" s="212" t="n"/>
-      <c r="C74" s="212" t="n"/>
+      <c r="C74" s="212" t="inlineStr">
+        <is>
+          <t>6.25</t>
+        </is>
+      </c>
       <c r="D74" s="25" t="n"/>
-      <c r="E74" s="26" t="n"/>
+      <c r="E74" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F74" s="27" t="n"/>
       <c r="G74" s="210" t="n"/>
       <c r="H74" s="320" t="n"/>
@@ -33619,7 +34543,11 @@
       <c r="N74" s="210" t="n"/>
       <c r="O74" s="320" t="n"/>
       <c r="P74" s="319" t="n"/>
-      <c r="Q74" s="31" t="n"/>
+      <c r="Q74" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 14:30-20:45</t>
+        </is>
+      </c>
       <c r="R74" s="32" t="n"/>
       <c r="S74" s="32" t="n"/>
       <c r="T74" s="32" t="n"/>
@@ -38561,11 +39489,23 @@
       <c r="AF62" s="33" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="24" t="n"/>
+      <c r="A63" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
       <c r="B63" s="212" t="n"/>
-      <c r="C63" s="212" t="n"/>
+      <c r="C63" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
       <c r="D63" s="25" t="n"/>
-      <c r="E63" s="26" t="n"/>
+      <c r="E63" s="26" t="inlineStr">
+        <is>
+          <t>US NCL</t>
+        </is>
+      </c>
       <c r="F63" s="27" t="n"/>
       <c r="G63" s="210" t="n"/>
       <c r="H63" s="320" t="n"/>
@@ -38577,7 +39517,11 @@
       <c r="N63" s="210" t="n"/>
       <c r="O63" s="320" t="n"/>
       <c r="P63" s="319" t="n"/>
-      <c r="Q63" s="31" t="n"/>
+      <c r="Q63" s="31" t="inlineStr">
+        <is>
+          <t>US NCL 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R63" s="32" t="n"/>
       <c r="S63" s="32" t="n"/>
       <c r="T63" s="32" t="n"/>
@@ -38595,11 +39539,23 @@
       <c r="AF63" s="33" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" s="24" t="n"/>
+      <c r="A64" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-03</t>
+        </is>
+      </c>
       <c r="B64" s="212" t="n"/>
-      <c r="C64" s="212" t="n"/>
+      <c r="C64" s="212" t="inlineStr">
+        <is>
+          <t>8.50</t>
+        </is>
+      </c>
       <c r="D64" s="25" t="n"/>
-      <c r="E64" s="26" t="n"/>
+      <c r="E64" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F64" s="27" t="n"/>
       <c r="G64" s="210" t="n"/>
       <c r="H64" s="320" t="n"/>
@@ -38611,7 +39567,11 @@
       <c r="N64" s="210" t="n"/>
       <c r="O64" s="320" t="n"/>
       <c r="P64" s="319" t="n"/>
-      <c r="Q64" s="31" t="n"/>
+      <c r="Q64" s="31" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 13:30-22:00</t>
+        </is>
+      </c>
       <c r="R64" s="32" t="n"/>
       <c r="S64" s="32" t="n"/>
       <c r="T64" s="32" t="n"/>
@@ -38629,11 +39589,23 @@
       <c r="AF64" s="33" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="24" t="n"/>
+      <c r="A65" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-12</t>
+        </is>
+      </c>
       <c r="B65" s="212" t="n"/>
-      <c r="C65" s="212" t="n"/>
+      <c r="C65" s="212" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
       <c r="D65" s="25" t="n"/>
-      <c r="E65" s="26" t="n"/>
+      <c r="E65" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F65" s="27" t="n"/>
       <c r="G65" s="210" t="n"/>
       <c r="H65" s="320" t="n"/>
@@ -38645,7 +39617,11 @@
       <c r="N65" s="210" t="n"/>
       <c r="O65" s="320" t="n"/>
       <c r="P65" s="319" t="n"/>
-      <c r="Q65" s="31" t="n"/>
+      <c r="Q65" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 13:30-13:44</t>
+        </is>
+      </c>
       <c r="R65" s="32" t="n"/>
       <c r="S65" s="32" t="n"/>
       <c r="T65" s="32" t="n"/>
@@ -38663,11 +39639,23 @@
       <c r="AF65" s="33" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="24" t="n"/>
+      <c r="A66" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-16</t>
+        </is>
+      </c>
       <c r="B66" s="212" t="n"/>
-      <c r="C66" s="212" t="n"/>
+      <c r="C66" s="212" t="inlineStr">
+        <is>
+          <t>4.50</t>
+        </is>
+      </c>
       <c r="D66" s="25" t="n"/>
-      <c r="E66" s="26" t="n"/>
+      <c r="E66" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F66" s="27" t="n"/>
       <c r="G66" s="210" t="n"/>
       <c r="H66" s="320" t="n"/>
@@ -38679,7 +39667,11 @@
       <c r="N66" s="210" t="n"/>
       <c r="O66" s="320" t="n"/>
       <c r="P66" s="319" t="n"/>
-      <c r="Q66" s="31" t="n"/>
+      <c r="Q66" s="31" t="inlineStr">
+        <is>
+          <t>US Tardy 13:30-18:00</t>
+        </is>
+      </c>
       <c r="R66" s="32" t="n"/>
       <c r="S66" s="32" t="n"/>
       <c r="T66" s="32" t="n"/>
@@ -41370,11 +42362,23 @@
       <c r="AF50" s="319" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="24" t="n"/>
+      <c r="A51" s="24" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B51" s="212" t="n"/>
-      <c r="C51" s="212" t="n"/>
+      <c r="C51" s="212" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
       <c r="D51" s="25" t="n"/>
-      <c r="E51" s="26" t="n"/>
+      <c r="E51" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F51" s="27" t="n"/>
       <c r="G51" s="210" t="n"/>
       <c r="H51" s="320" t="n"/>
@@ -41386,7 +42390,11 @@
       <c r="N51" s="210" t="n"/>
       <c r="O51" s="320" t="n"/>
       <c r="P51" s="319" t="n"/>
-      <c r="Q51" s="153" t="n"/>
+      <c r="Q51" s="153" t="inlineStr">
+        <is>
+          <t>US Tardy 11:45-13:18</t>
+        </is>
+      </c>
       <c r="R51" s="320" t="n"/>
       <c r="S51" s="320" t="n"/>
       <c r="T51" s="320" t="n"/>
@@ -41404,11 +42412,23 @@
       <c r="AF51" s="319" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="24" t="n"/>
+      <c r="A52" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
       <c r="B52" s="212" t="n"/>
-      <c r="C52" s="212" t="n"/>
+      <c r="C52" s="212" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
       <c r="D52" s="25" t="n"/>
-      <c r="E52" s="26" t="n"/>
+      <c r="E52" s="26" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
       <c r="F52" s="27" t="n"/>
       <c r="G52" s="210" t="n"/>
       <c r="H52" s="320" t="n"/>
@@ -41420,7 +42440,11 @@
       <c r="N52" s="210" t="n"/>
       <c r="O52" s="320" t="n"/>
       <c r="P52" s="319" t="n"/>
-      <c r="Q52" s="153" t="n"/>
+      <c r="Q52" s="153" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 11:45-22:00</t>
+        </is>
+      </c>
       <c r="R52" s="320" t="n"/>
       <c r="S52" s="320" t="n"/>
       <c r="T52" s="320" t="n"/>
@@ -41438,11 +42462,23 @@
       <c r="AF52" s="319" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="24" t="n"/>
+      <c r="A53" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-14</t>
+        </is>
+      </c>
       <c r="B53" s="212" t="n"/>
-      <c r="C53" s="212" t="n"/>
+      <c r="C53" s="212" t="inlineStr">
+        <is>
+          <t>4.85</t>
+        </is>
+      </c>
       <c r="D53" s="25" t="n"/>
-      <c r="E53" s="26" t="n"/>
+      <c r="E53" s="26" t="inlineStr">
+        <is>
+          <t>US Partial</t>
+        </is>
+      </c>
       <c r="F53" s="27" t="n"/>
       <c r="G53" s="210" t="n"/>
       <c r="H53" s="320" t="n"/>
@@ -41454,7 +42490,11 @@
       <c r="N53" s="210" t="n"/>
       <c r="O53" s="320" t="n"/>
       <c r="P53" s="319" t="n"/>
-      <c r="Q53" s="153" t="n"/>
+      <c r="Q53" s="153" t="inlineStr">
+        <is>
+          <t>US Partial 17:09-22:00</t>
+        </is>
+      </c>
       <c r="R53" s="320" t="n"/>
       <c r="S53" s="320" t="n"/>
       <c r="T53" s="320" t="n"/>
@@ -41472,11 +42512,23 @@
       <c r="AF53" s="319" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="24" t="n"/>
+      <c r="A54" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-14</t>
+        </is>
+      </c>
       <c r="B54" s="212" t="n"/>
-      <c r="C54" s="212" t="n"/>
+      <c r="C54" s="212" t="inlineStr">
+        <is>
+          <t>1.08</t>
+        </is>
+      </c>
       <c r="D54" s="25" t="n"/>
-      <c r="E54" s="26" t="n"/>
+      <c r="E54" s="26" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
       <c r="F54" s="27" t="n"/>
       <c r="G54" s="210" t="n"/>
       <c r="H54" s="320" t="n"/>
@@ -41488,7 +42540,11 @@
       <c r="N54" s="210" t="n"/>
       <c r="O54" s="320" t="n"/>
       <c r="P54" s="319" t="n"/>
-      <c r="Q54" s="153" t="n"/>
+      <c r="Q54" s="153" t="inlineStr">
+        <is>
+          <t>US Tardy 11:45-12:50</t>
+        </is>
+      </c>
       <c r="R54" s="320" t="n"/>
       <c r="S54" s="320" t="n"/>
       <c r="T54" s="320" t="n"/>
@@ -41506,11 +42562,23 @@
       <c r="AF54" s="319" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="24" t="n"/>
+      <c r="A55" s="24" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
       <c r="B55" s="212" t="n"/>
-      <c r="C55" s="212" t="n"/>
+      <c r="C55" s="212" t="inlineStr">
+        <is>
+          <t>3.20</t>
+        </is>
+      </c>
       <c r="D55" s="25" t="n"/>
-      <c r="E55" s="26" t="n"/>
+      <c r="E55" s="26" t="inlineStr">
+        <is>
+          <t>US Partial</t>
+        </is>
+      </c>
       <c r="F55" s="27" t="n"/>
       <c r="G55" s="210" t="n"/>
       <c r="H55" s="320" t="n"/>
@@ -41522,7 +42590,11 @@
       <c r="N55" s="210" t="n"/>
       <c r="O55" s="320" t="n"/>
       <c r="P55" s="319" t="n"/>
-      <c r="Q55" s="153" t="n"/>
+      <c r="Q55" s="153" t="inlineStr">
+        <is>
+          <t>US Partial 18:48-22:00</t>
+        </is>
+      </c>
       <c r="R55" s="320" t="n"/>
       <c r="S55" s="320" t="n"/>
       <c r="T55" s="320" t="n"/>
@@ -42507,7 +43579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK95"/>
+  <dimension ref="A1:AK101"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="Q82" sqref="Q82"/>
@@ -46461,6 +47533,138 @@
         </is>
       </c>
       <c r="Q95" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 09:00-19:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2023-12-16</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-09:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2023-12-23</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-09:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-10:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2024-01-06</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-09:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2024-01-13</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>US Tardy 09:00-09:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
+      <c r="Q101" t="inlineStr">
         <is>
           <t>US Absent Unplanned 09:00-19:15</t>
         </is>
@@ -46811,7 +48015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DL77"/>
+  <dimension ref="A1:DL86"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="Q51" sqref="Q51:AF178"/>
@@ -52129,6 +53333,204 @@
         </is>
       </c>
       <c r="Q77" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:00-20:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2023-12-15</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-11:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:00-20:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2023-12-26</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>8.97</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>US Partial</t>
+        </is>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>US Partial 11:17-20:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2023-12-30</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-10:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>5.33</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-15:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2024-01-02</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-10:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2024-01-05</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>3.92</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>US Tardy</t>
+        </is>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>US Tardy 10:00-13:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned 10:00-20:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>10.25</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>US Absent Unplanned</t>
+        </is>
+      </c>
+      <c r="Q86" t="inlineStr">
         <is>
           <t>US Absent Unplanned 10:00-20:15</t>
         </is>

</xml_diff>